<commit_message>
Platform reading of Comparison, Advance Pivot, Ballot box and Segmentation report added.
</commit_message>
<xml_diff>
--- a/Engage/Engage-Performance/src/main/resources/excelfiles/Engage_PlatformReadings.xlsx
+++ b/Engage/Engage-Performance/src/main/resources/excelfiles/Engage_PlatformReadings.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C8A616-C5FD-45D8-8E9E-66A839EFEF60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001CD36A-F26D-4B45-A333-45950F09F827}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="201">
   <si>
     <t>Environment</t>
   </si>
@@ -448,9 +448,6 @@
     <t>Segment 1 name</t>
   </si>
   <si>
-    <t xml:space="preserve"> Statistical Report - Segment Answer Options not present on page.</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
@@ -514,13 +511,121 @@
     <t>Step 7 : Select Filter</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Engagement - Additional Question Toggle not present on page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Engagement - Composition Analysis Toggle not present on page.</t>
+    <t>PlatformReadings_TC20</t>
+  </si>
+  <si>
+    <t>Comparison Report (2 Dataset)</t>
+  </si>
+  <si>
+    <t>Step 1:Select Survey Question</t>
+  </si>
+  <si>
+    <t>Step 3: Select Survey Dataset (Apply condition on both)</t>
+  </si>
+  <si>
+    <t>Step 4: Select Report properties</t>
+  </si>
+  <si>
+    <t>datasetCount</t>
+  </si>
+  <si>
+    <t>Overall Assessment: I am proud to work for Al Hilal Bank/~/Working Conditions: My work area is physically comfortable.</t>
+  </si>
+  <si>
+    <t>is/~/is</t>
+  </si>
+  <si>
+    <t>5/~/5</t>
+  </si>
+  <si>
+    <t>2 Datasets</t>
+  </si>
+  <si>
+    <t>Comparison Report (5 Dataset)</t>
+  </si>
+  <si>
+    <t>5 Datasets</t>
+  </si>
+  <si>
+    <t>Overall Assessment: I am proud to work for Al Hilal Bank/~/Working Conditions: My work area is physically comfortable./~/Shared Values with Al Hilal Bank: Al Hilal Bank cares about the same things that I care about./~/Quality of Al Hilal Bank’s Products/Services: I am proud of the quality of Al Hilal Bank's products/services./~/Adaptability of Immediate Supervisor: My supervisor is good at making changes when they are necessary.</t>
+  </si>
+  <si>
+    <t>is/~/is/~/is/~/is/~/is</t>
+  </si>
+  <si>
+    <t>5/~/5/~/5/~/5/~/5</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC21</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC22</t>
+  </si>
+  <si>
+    <t>Ballot Box Report</t>
+  </si>
+  <si>
+    <t>Step 1 : Specify Internal IP Address</t>
+  </si>
+  <si>
+    <t>Step 2 : Number of Duplicate Allowed</t>
+  </si>
+  <si>
+    <t>Step 3: Data Review</t>
+  </si>
+  <si>
+    <t>Do not put IP</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC23</t>
+  </si>
+  <si>
+    <t>Advance Pivot Report</t>
+  </si>
+  <si>
+    <t>Step 1 : Select segmentation question</t>
+  </si>
+  <si>
+    <t>Step 2 : Select Survey Question</t>
+  </si>
+  <si>
+    <t>Step 3: Merge answer option</t>
+  </si>
+  <si>
+    <t>Step 5 : Select Filter</t>
+  </si>
+  <si>
+    <t>toEmail</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC24</t>
+  </si>
+  <si>
+    <t>Segmentation Report</t>
+  </si>
+  <si>
+    <t>Step 1: Select Segmentation Question</t>
+  </si>
+  <si>
+    <t>Step 2 : Select Survey Questions</t>
+  </si>
+  <si>
+    <t>Step 5: Comparison Segment Data</t>
+  </si>
+  <si>
+    <t>Q1(a). I am proud to work for Al Hilal Bank</t>
+  </si>
+  <si>
+    <t>ggolatkar@zarca.com</t>
+  </si>
+  <si>
+    <t>Step 6 : Customize Cover Page</t>
+  </si>
+  <si>
+    <t>Step 7 : Email Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Did not find the option containing text Q1(a). I am proud to work for Al Hilal Bank</t>
   </si>
 </sst>
 </file>
@@ -528,7 +633,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -574,158 +679,29 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -739,7 +715,7 @@
       <color indexed="12"/>
     </font>
   </fonts>
-  <fills count="96">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -768,7 +744,7 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
+      <patternFill patternType="solid">
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
@@ -778,408 +754,13 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -1259,7 +840,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1273,66 +854,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="17" fillId="41" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="19" fillId="43" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="19" fillId="45" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="19" fillId="47" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="21" fillId="49" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="21" fillId="51" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="21" fillId="53" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="23" fillId="55" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="23" fillId="57" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="23" fillId="59" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="25" fillId="61" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="25" fillId="63" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="25" fillId="65" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="27" fillId="67" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="27" fillId="69" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="27" fillId="71" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="29" fillId="73" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="29" fillId="75" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="29" fillId="77" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="31" fillId="79" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="31" fillId="81" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="31" fillId="83" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="33" fillId="85" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="33" fillId="87" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="33" fillId="89" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="35" fillId="91" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="35" fillId="93" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="35" fillId="95" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1767,10 +1297,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B22B77-F9A0-48CA-B95A-663324812831}">
-  <dimension ref="A1:AQ20"/>
+  <dimension ref="A1:AS25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1785,13 +1315,10 @@
     <col min="8" max="8" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="11" max="19" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="20" max="22" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="23" max="39" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="40" max="42" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="11" max="44" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -1850,13 +1377,13 @@
         <v>51</v>
       </c>
       <c r="T1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="U1" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="V1" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="W1" s="3" t="s">
         <v>59</v>
@@ -1910,19 +1437,25 @@
         <v>140</v>
       </c>
       <c r="AN1" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AO1" s="3" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="AP1" s="3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="AQ1" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="AS1" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:43" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -1946,7 +1479,7 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="69" t="s">
+      <c r="J2" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K2" s="5"/>
@@ -1997,9 +1530,11 @@
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
       <c r="AP2" s="1"/>
-      <c r="AQ2" s="4"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="4"/>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -2023,7 +1558,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="69" t="s">
+      <c r="J3" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K3" s="5"/>
@@ -2072,9 +1607,11 @@
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
       <c r="AP3" s="1"/>
-      <c r="AQ3" s="4"/>
+      <c r="AQ3" s="1"/>
+      <c r="AR3" s="1"/>
+      <c r="AS3" s="4"/>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -2098,7 +1635,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="69" t="s">
+      <c r="J4" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K4" s="5"/>
@@ -2147,9 +1684,11 @@
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
-      <c r="AQ4" s="4"/>
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="1"/>
+      <c r="AS4" s="4"/>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -2173,7 +1712,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="69" t="s">
+      <c r="J5" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="5"/>
@@ -2222,9 +1761,11 @@
       <c r="AN5" s="1"/>
       <c r="AO5" s="1"/>
       <c r="AP5" s="1"/>
-      <c r="AQ5" s="4"/>
+      <c r="AQ5" s="1"/>
+      <c r="AR5" s="1"/>
+      <c r="AS5" s="4"/>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -2248,7 +1789,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="69" t="s">
+      <c r="J6" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K6" s="5"/>
@@ -2313,9 +1854,11 @@
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
       <c r="AP6" s="1"/>
-      <c r="AQ6" s="4"/>
+      <c r="AQ6" s="1"/>
+      <c r="AR6" s="1"/>
+      <c r="AS6" s="4"/>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>72</v>
       </c>
@@ -2339,7 +1882,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="6"/>
-      <c r="J7" s="69" t="s">
+      <c r="J7" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K7" s="5"/>
@@ -2404,9 +1947,11 @@
       <c r="AN7" s="1"/>
       <c r="AO7" s="1"/>
       <c r="AP7" s="1"/>
-      <c r="AQ7" s="4"/>
+      <c r="AQ7" s="1"/>
+      <c r="AR7" s="1"/>
+      <c r="AS7" s="4"/>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>75</v>
       </c>
@@ -2430,7 +1975,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="69" t="s">
+      <c r="J8" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K8" s="5"/>
@@ -2481,9 +2026,11 @@
       <c r="AN8" s="1"/>
       <c r="AO8" s="1"/>
       <c r="AP8" s="1"/>
-      <c r="AQ8" s="4"/>
+      <c r="AQ8" s="1"/>
+      <c r="AR8" s="1"/>
+      <c r="AS8" s="4"/>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>84</v>
       </c>
@@ -2507,7 +2054,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="69" t="s">
+      <c r="J9" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K9" s="5"/>
@@ -2560,9 +2107,11 @@
       <c r="AN9" s="1"/>
       <c r="AO9" s="1"/>
       <c r="AP9" s="1"/>
-      <c r="AQ9" s="4"/>
+      <c r="AQ9" s="1"/>
+      <c r="AR9" s="1"/>
+      <c r="AS9" s="4"/>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>89</v>
       </c>
@@ -2586,7 +2135,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="69" t="s">
+      <c r="J10" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K10" s="5"/>
@@ -2639,9 +2188,11 @@
       <c r="AN10" s="1"/>
       <c r="AO10" s="1"/>
       <c r="AP10" s="1"/>
-      <c r="AQ10" s="4"/>
+      <c r="AQ10" s="1"/>
+      <c r="AR10" s="1"/>
+      <c r="AS10" s="4"/>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>92</v>
       </c>
@@ -2665,7 +2216,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="69" t="s">
+      <c r="J11" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K11" s="5"/>
@@ -2718,9 +2269,11 @@
       <c r="AN11" s="1"/>
       <c r="AO11" s="1"/>
       <c r="AP11" s="1"/>
-      <c r="AQ11" s="4"/>
+      <c r="AQ11" s="1"/>
+      <c r="AR11" s="1"/>
+      <c r="AS11" s="4"/>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>95</v>
       </c>
@@ -2744,7 +2297,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="69" t="s">
+      <c r="J12" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K12" s="5"/>
@@ -2797,9 +2350,11 @@
       <c r="AN12" s="1"/>
       <c r="AO12" s="1"/>
       <c r="AP12" s="1"/>
-      <c r="AQ12" s="4"/>
+      <c r="AQ12" s="1"/>
+      <c r="AR12" s="1"/>
+      <c r="AS12" s="4"/>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>104</v>
       </c>
@@ -2823,7 +2378,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="69" t="s">
+      <c r="J13" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K13" s="5"/>
@@ -2878,9 +2433,11 @@
       <c r="AN13" s="7"/>
       <c r="AO13" s="7"/>
       <c r="AP13" s="7"/>
-      <c r="AQ13" s="4"/>
+      <c r="AQ13" s="7"/>
+      <c r="AR13" s="7"/>
+      <c r="AS13" s="4"/>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>107</v>
       </c>
@@ -2904,7 +2461,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="69" t="s">
+      <c r="J14" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K14" s="5"/>
@@ -2959,9 +2516,11 @@
       <c r="AN14" s="8"/>
       <c r="AO14" s="8"/>
       <c r="AP14" s="8"/>
-      <c r="AQ14" s="4"/>
+      <c r="AQ14" s="8"/>
+      <c r="AR14" s="8"/>
+      <c r="AS14" s="4"/>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>118</v>
       </c>
@@ -2985,7 +2544,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="69" t="s">
+      <c r="J15" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K15" s="5"/>
@@ -3034,9 +2593,11 @@
       <c r="AN15" s="8"/>
       <c r="AO15" s="8"/>
       <c r="AP15" s="8"/>
-      <c r="AQ15" s="4"/>
+      <c r="AQ15" s="8"/>
+      <c r="AR15" s="8"/>
+      <c r="AS15" s="4"/>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>121</v>
       </c>
@@ -3060,7 +2621,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="69" t="s">
+      <c r="J16" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K16" s="5"/>
@@ -3101,9 +2662,11 @@
       <c r="AN16" s="8"/>
       <c r="AO16" s="8"/>
       <c r="AP16" s="8"/>
-      <c r="AQ16" s="4"/>
+      <c r="AQ16" s="8"/>
+      <c r="AR16" s="8"/>
+      <c r="AS16" s="4"/>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>123</v>
       </c>
@@ -3127,7 +2690,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="69" t="s">
+      <c r="J17" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K17" s="5"/>
@@ -3178,9 +2741,11 @@
       <c r="AN17" s="8"/>
       <c r="AO17" s="8"/>
       <c r="AP17" s="8"/>
-      <c r="AQ17" s="4"/>
+      <c r="AQ17" s="8"/>
+      <c r="AR17" s="8"/>
+      <c r="AS17" s="4"/>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>128</v>
       </c>
@@ -3204,12 +2769,10 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="69" t="s">
+      <c r="J18" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="K18" s="5" t="s">
-        <v>141</v>
-      </c>
+      <c r="K18" s="5"/>
       <c r="L18" s="5" t="s">
         <v>47</v>
       </c>
@@ -3259,9 +2822,11 @@
       <c r="AN18" s="8"/>
       <c r="AO18" s="8"/>
       <c r="AP18" s="8"/>
-      <c r="AQ18" s="4"/>
+      <c r="AQ18" s="8"/>
+      <c r="AR18" s="8"/>
+      <c r="AS18" s="4"/>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>131</v>
       </c>
@@ -3285,7 +2850,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="69" t="s">
+      <c r="J19" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K19" s="5"/>
@@ -3344,14 +2909,16 @@
       <c r="AN19" s="1"/>
       <c r="AO19" s="1"/>
       <c r="AP19" s="1"/>
-      <c r="AQ19" s="4"/>
+      <c r="AQ19" s="1"/>
+      <c r="AR19" s="1"/>
+      <c r="AS19" s="4"/>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
@@ -3366,48 +2933,46 @@
         <v>43</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="67" t="s">
-        <v>142</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>164</v>
-      </c>
+      <c r="J20" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="K20" s="5"/>
       <c r="L20" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M20" s="5">
         <v>859</v>
       </c>
       <c r="N20" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="O20" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="P20" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="Q20" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="Q20" s="1" t="s">
+      <c r="R20" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="R20" s="1" t="s">
+      <c r="S20" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="S20" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="T20" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="U20" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="V20" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
@@ -3429,17 +2994,443 @@
       <c r="AN20" s="1">
         <v>1000</v>
       </c>
-      <c r="AO20" s="1" t="s">
+      <c r="AO20" s="1"/>
+      <c r="AP20" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AQ20" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="AP20" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="AQ20" s="4"/>
+      <c r="AR20" s="1"/>
+      <c r="AS20" s="4"/>
+    </row>
+    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M21" s="5">
+        <v>527</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1"/>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="7"/>
+      <c r="AI21" s="8"/>
+      <c r="AJ21" s="8"/>
+      <c r="AK21" s="1"/>
+      <c r="AL21" s="1"/>
+      <c r="AM21" s="1"/>
+      <c r="AN21" s="1"/>
+      <c r="AO21" s="1">
+        <v>2</v>
+      </c>
+      <c r="AP21" s="1"/>
+      <c r="AQ21" s="1"/>
+      <c r="AR21" s="1"/>
+      <c r="AS21" s="4"/>
+    </row>
+    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M22" s="5">
+        <v>527</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="7"/>
+      <c r="AI22" s="8"/>
+      <c r="AJ22" s="8"/>
+      <c r="AK22" s="1"/>
+      <c r="AL22" s="1"/>
+      <c r="AM22" s="1"/>
+      <c r="AN22" s="1"/>
+      <c r="AO22" s="1">
+        <v>5</v>
+      </c>
+      <c r="AP22" s="1"/>
+      <c r="AQ22" s="1"/>
+      <c r="AR22" s="1"/>
+      <c r="AS22" s="4"/>
+    </row>
+    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="M23" s="5">
+        <v>14</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+      <c r="AF23" s="1"/>
+      <c r="AG23" s="1"/>
+      <c r="AH23" s="7"/>
+      <c r="AI23" s="8"/>
+      <c r="AJ23" s="8"/>
+      <c r="AK23" s="1"/>
+      <c r="AL23" s="1"/>
+      <c r="AM23" s="1"/>
+      <c r="AN23" s="1">
+        <v>2</v>
+      </c>
+      <c r="AO23" s="1"/>
+      <c r="AP23" s="1"/>
+      <c r="AQ23" s="1"/>
+      <c r="AR23" s="1"/>
+      <c r="AS23" s="4"/>
+    </row>
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M24" s="5">
+        <v>527</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="1"/>
+      <c r="AF24" s="1"/>
+      <c r="AG24" s="1"/>
+      <c r="AH24" s="7"/>
+      <c r="AI24" s="8"/>
+      <c r="AJ24" s="8"/>
+      <c r="AK24" s="1"/>
+      <c r="AL24" s="1"/>
+      <c r="AM24" s="1"/>
+      <c r="AN24" s="1"/>
+      <c r="AO24" s="1"/>
+      <c r="AP24" s="1"/>
+      <c r="AQ24" s="1"/>
+      <c r="AR24" s="1"/>
+      <c r="AS24" s="4"/>
+    </row>
+    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M25" s="5">
+        <v>527</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="V25" s="1"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+      <c r="AF25" s="1"/>
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="7"/>
+      <c r="AI25" s="8"/>
+      <c r="AJ25" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="AK25" s="1"/>
+      <c r="AL25" s="1"/>
+      <c r="AM25" s="1"/>
+      <c r="AN25" s="1"/>
+      <c r="AO25" s="1"/>
+      <c r="AP25" s="1"/>
+      <c r="AQ25" s="1"/>
+      <c r="AR25" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AS25" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="AR25" r:id="rId1" xr:uid="{FCAF826B-C13B-457E-A6AA-2797C89CE965}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Zarca DMX Reading completed and implementing Webdriver manager API in engage performance suite.
</commit_message>
<xml_diff>
--- a/Engage/Engage-Performance/src/main/resources/excelfiles/Engage_PlatformReadings.xlsx
+++ b/Engage/Engage-Performance/src/main/resources/excelfiles/Engage_PlatformReadings.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001CD36A-F26D-4B45-A333-45950F09F827}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F3861A-F49D-4FC8-A44D-90AEB0970390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4110" yWindow="3045" windowWidth="15375" windowHeight="7875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="356">
   <si>
     <t>Environment</t>
   </si>
@@ -448,184 +448,649 @@
     <t>Segment 1 name</t>
   </si>
   <si>
+    <t>PlatformReadings_TC19</t>
+  </si>
+  <si>
+    <t>Engagement Report</t>
+  </si>
+  <si>
+    <t>Engagement questions</t>
+  </si>
+  <si>
+    <t>Nmax</t>
+  </si>
+  <si>
+    <t>Driver questions</t>
+  </si>
+  <si>
+    <t>Step 1 : Report Details</t>
+  </si>
+  <si>
+    <t>Step 2 : Identify Engagement Questions (8 Question)</t>
+  </si>
+  <si>
+    <t>Step 3: Identify Driver Questions (8 Question)</t>
+  </si>
+  <si>
+    <t>Step 4 : Specify Additional Questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 5 Composition Analysis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 6 : Segmentation Report </t>
+  </si>
+  <si>
+    <t>Step 7</t>
+  </si>
+  <si>
+    <t>Step 8</t>
+  </si>
+  <si>
+    <t>Generate Report[PPT]</t>
+  </si>
+  <si>
+    <t>Generate Report[Excel]</t>
+  </si>
+  <si>
+    <t>2012 Staff Engagement Survey LAUNCH FROM K12_GPISDcs</t>
+  </si>
+  <si>
+    <t>Step 9</t>
+  </si>
+  <si>
+    <t>Step 7 : Select Filter</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC20</t>
+  </si>
+  <si>
+    <t>Comparison Report (2 Dataset)</t>
+  </si>
+  <si>
+    <t>Step 1:Select Survey Question</t>
+  </si>
+  <si>
+    <t>Step 3: Select Survey Dataset (Apply condition on both)</t>
+  </si>
+  <si>
+    <t>Step 4: Select Report properties</t>
+  </si>
+  <si>
+    <t>datasetCount</t>
+  </si>
+  <si>
+    <t>Overall Assessment: I am proud to work for Al Hilal Bank/~/Working Conditions: My work area is physically comfortable.</t>
+  </si>
+  <si>
+    <t>is/~/is</t>
+  </si>
+  <si>
+    <t>5/~/5</t>
+  </si>
+  <si>
+    <t>2 Datasets</t>
+  </si>
+  <si>
+    <t>Comparison Report (5 Dataset)</t>
+  </si>
+  <si>
+    <t>5 Datasets</t>
+  </si>
+  <si>
+    <t>Overall Assessment: I am proud to work for Al Hilal Bank/~/Working Conditions: My work area is physically comfortable./~/Shared Values with Al Hilal Bank: Al Hilal Bank cares about the same things that I care about./~/Quality of Al Hilal Bank’s Products/Services: I am proud of the quality of Al Hilal Bank's products/services./~/Adaptability of Immediate Supervisor: My supervisor is good at making changes when they are necessary.</t>
+  </si>
+  <si>
+    <t>is/~/is/~/is/~/is/~/is</t>
+  </si>
+  <si>
+    <t>5/~/5/~/5/~/5/~/5</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC21</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC22</t>
+  </si>
+  <si>
+    <t>Ballot Box Report</t>
+  </si>
+  <si>
+    <t>Step 1 : Specify Internal IP Address</t>
+  </si>
+  <si>
+    <t>Step 2 : Number of Duplicate Allowed</t>
+  </si>
+  <si>
+    <t>Step 3: Data Review</t>
+  </si>
+  <si>
+    <t>Do not put IP</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC23</t>
+  </si>
+  <si>
+    <t>Advance Pivot Report</t>
+  </si>
+  <si>
+    <t>Step 1 : Select segmentation question</t>
+  </si>
+  <si>
+    <t>Step 2 : Select Survey Question</t>
+  </si>
+  <si>
+    <t>Step 3: Merge answer option</t>
+  </si>
+  <si>
+    <t>Step 5 : Select Filter</t>
+  </si>
+  <si>
+    <t>toEmail</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC24</t>
+  </si>
+  <si>
+    <t>Segmentation Report</t>
+  </si>
+  <si>
+    <t>Step 1: Select Segmentation Question</t>
+  </si>
+  <si>
+    <t>Step 2 : Select Survey Questions</t>
+  </si>
+  <si>
+    <t>Step 5: Comparison Segment Data</t>
+  </si>
+  <si>
+    <t>Q1(a). I am proud to work for Al Hilal Bank</t>
+  </si>
+  <si>
+    <t>ggolatkar@zarca.com</t>
+  </si>
+  <si>
+    <t>Step 6 : Customize Cover Page</t>
+  </si>
+  <si>
+    <t>Step 7 : Email Report</t>
+  </si>
+  <si>
+    <t>BETA</t>
+  </si>
+  <si>
+    <t>https://beta.zarca.com/static/Register/clientlogin.aspx</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC25</t>
+  </si>
+  <si>
+    <t>DMX</t>
+  </si>
+  <si>
+    <t>DM Home Page</t>
+  </si>
+  <si>
+    <t>rohan_test</t>
+  </si>
+  <si>
+    <t>Welcome@1234</t>
+  </si>
+  <si>
+    <t>DMX Manual Readings</t>
+  </si>
+  <si>
+    <t>Home - DM page</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC26</t>
+  </si>
+  <si>
+    <t>Invitation Wizard (1000 records via list)</t>
+  </si>
+  <si>
+    <t>emailtemplate</t>
+  </si>
+  <si>
+    <t>DNT - Automation DMX Reading</t>
+  </si>
+  <si>
+    <t>Step 1: Select Type Of Survey URL To Be Sent</t>
+  </si>
+  <si>
+    <t>Step 2: Select Email Message</t>
+  </si>
+  <si>
+    <t>Step 3: Select source of email addresses</t>
+  </si>
+  <si>
+    <t>Step 4: Select List of 1000</t>
+  </si>
+  <si>
+    <t>DNT- Automation DMX 1000 list</t>
+  </si>
+  <si>
+    <t>selectlist</t>
+  </si>
+  <si>
+    <t>Step 5 : Mail Merge</t>
+  </si>
+  <si>
+    <t>Step 6: Pre-Populate Survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quick send button not present on page.</t>
+  </si>
+  <si>
+    <t>Email Address/~/First Name/~/Last Name</t>
+  </si>
+  <si>
+    <t>prepopdd</t>
+  </si>
+  <si>
+    <t>Step 7: Prepop mismatch</t>
+  </si>
+  <si>
+    <t>Step 9: Send Now</t>
+  </si>
+  <si>
+    <t>Step 8: Send or Schedule Invitation</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC27</t>
+  </si>
+  <si>
+    <t>Invitation Wizard (1000 records via file)</t>
+  </si>
+  <si>
+    <t>Step 4 : Mail Merge</t>
+  </si>
+  <si>
+    <t>Step 5: Pre-Populate Survey</t>
+  </si>
+  <si>
+    <t>Step 6: Prepop mismatch</t>
+  </si>
+  <si>
+    <t>Step 7: Send or Schedule Invitation</t>
+  </si>
+  <si>
+    <t>Step 8: Send Now</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>Column1/~/Column2/~/Column3</t>
+  </si>
+  <si>
+    <t>DNT- Automation DMX 1000 list.xls</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC28</t>
+  </si>
+  <si>
+    <t>Invitation Wizard (1000 records Type Manually)</t>
+  </si>
+  <si>
+    <t>Type Manually 1000 records.txt</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC29</t>
+  </si>
+  <si>
+    <t>Quick Send (999 records)</t>
+  </si>
+  <si>
+    <t>DNT - Automation DMX Reading - Quick Send</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Type Manually 999 records.txt</t>
+  </si>
+  <si>
+    <t>Step 1: Send 999 records via Quick Send</t>
+  </si>
+  <si>
+    <t>mapValues</t>
+  </si>
+  <si>
+    <t>emailaddcol</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>List Creation (Import 1000 records with 3 attributes)</t>
+  </si>
+  <si>
+    <t>Step 2: Define source (Import file of 1 k records)</t>
+  </si>
+  <si>
+    <t>Step 1: List Manager Main page(account should have 30 list with 5000 records each)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 3: Populate List </t>
+  </si>
+  <si>
+    <t>Step 4 : List Manager Main page  after List Creation</t>
+  </si>
+  <si>
+    <t>Contact List Creation - 1000 Records.xls</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC30</t>
+  </si>
+  <si>
+    <t>Email Address/~/First Name/~/Last Name/~/Company</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>PlatformReadings_TC19</t>
-  </si>
-  <si>
-    <t>Engagement Report</t>
-  </si>
-  <si>
-    <t>Engagement questions</t>
-  </si>
-  <si>
-    <t>Nmax</t>
-  </si>
-  <si>
-    <t>I am proud to work at my school;Teaching gives me a feeling of accomplishment;Overall, I am satisfied with teaching;My current teaching duties are interesting;I am motivated to contribute more than what is expected of me at this school;I am not planning on leaving this school;I would feel comfortable referring a good friend to teach at this school;Overall, I enjoy working for this school’s principal</t>
-  </si>
-  <si>
-    <t>The school administrators make good decisions for the school overall;I enjoy the relationships I have with the school administrators;The classrooms where I teach are physically comfortable;My physical safety is protected at school;The school policies meet my needs as a teacher;The school supplies all the resources that I need to effectively teach my students;I fill a necessary role in the learning and growth of my students;I am a positive influence on my students</t>
-  </si>
-  <si>
-    <t>Driver questions</t>
-  </si>
-  <si>
-    <t>Step 1 : Report Details</t>
-  </si>
-  <si>
-    <t>Step 2 : Identify Engagement Questions (8 Question)</t>
-  </si>
-  <si>
-    <t>Step 3: Identify Driver Questions (8 Question)</t>
-  </si>
-  <si>
-    <t>Step 4 : Specify Additional Questions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step 5 Composition Analysis </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step 6 : Segmentation Report </t>
-  </si>
-  <si>
-    <t>Step 7</t>
-  </si>
-  <si>
-    <t>Step 8</t>
-  </si>
-  <si>
-    <t>Generate Report[PPT]</t>
-  </si>
-  <si>
-    <t>Generate Report[Excel]</t>
-  </si>
-  <si>
-    <t>2012 Staff Engagement Survey LAUNCH FROM K12_GPISDcs</t>
-  </si>
-  <si>
-    <t>Step 9</t>
-  </si>
-  <si>
-    <t>Step 7 : Select Filter</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC20</t>
-  </si>
-  <si>
-    <t>Comparison Report (2 Dataset)</t>
-  </si>
-  <si>
-    <t>Step 1:Select Survey Question</t>
-  </si>
-  <si>
-    <t>Step 3: Select Survey Dataset (Apply condition on both)</t>
-  </si>
-  <si>
-    <t>Step 4: Select Report properties</t>
-  </si>
-  <si>
-    <t>datasetCount</t>
-  </si>
-  <si>
-    <t>Overall Assessment: I am proud to work for Al Hilal Bank/~/Working Conditions: My work area is physically comfortable.</t>
-  </si>
-  <si>
-    <t>is/~/is</t>
-  </si>
-  <si>
-    <t>5/~/5</t>
-  </si>
-  <si>
-    <t>2 Datasets</t>
-  </si>
-  <si>
-    <t>Comparison Report (5 Dataset)</t>
-  </si>
-  <si>
-    <t>5 Datasets</t>
-  </si>
-  <si>
-    <t>Overall Assessment: I am proud to work for Al Hilal Bank/~/Working Conditions: My work area is physically comfortable./~/Shared Values with Al Hilal Bank: Al Hilal Bank cares about the same things that I care about./~/Quality of Al Hilal Bank’s Products/Services: I am proud of the quality of Al Hilal Bank's products/services./~/Adaptability of Immediate Supervisor: My supervisor is good at making changes when they are necessary.</t>
-  </si>
-  <si>
-    <t>is/~/is/~/is/~/is/~/is</t>
-  </si>
-  <si>
-    <t>5/~/5/~/5/~/5/~/5</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC21</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC22</t>
-  </si>
-  <si>
-    <t>Ballot Box Report</t>
-  </si>
-  <si>
-    <t>Step 1 : Specify Internal IP Address</t>
-  </si>
-  <si>
-    <t>Step 2 : Number of Duplicate Allowed</t>
-  </si>
-  <si>
-    <t>Step 3: Data Review</t>
-  </si>
-  <si>
-    <t>Do not put IP</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC23</t>
-  </si>
-  <si>
-    <t>Advance Pivot Report</t>
-  </si>
-  <si>
-    <t>Step 1 : Select segmentation question</t>
-  </si>
-  <si>
-    <t>Step 2 : Select Survey Question</t>
-  </si>
-  <si>
-    <t>Step 3: Merge answer option</t>
-  </si>
-  <si>
-    <t>Step 5 : Select Filter</t>
-  </si>
-  <si>
-    <t>toEmail</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC24</t>
-  </si>
-  <si>
-    <t>Segmentation Report</t>
-  </si>
-  <si>
-    <t>Step 1: Select Segmentation Question</t>
-  </si>
-  <si>
-    <t>Step 2 : Select Survey Questions</t>
-  </si>
-  <si>
-    <t>Step 5: Comparison Segment Data</t>
-  </si>
-  <si>
-    <t>Q1(a). I am proud to work for Al Hilal Bank</t>
-  </si>
-  <si>
-    <t>ggolatkar@zarca.com</t>
-  </si>
-  <si>
-    <t>Step 6 : Customize Cover Page</t>
-  </si>
-  <si>
-    <t>Step 7 : Email Report</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Did not find the option containing text Q1(a). I am proud to work for Al Hilal Bank</t>
+    <t>Step 5: Delete Same List</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC31</t>
+  </si>
+  <si>
+    <t>Offline invites for 999  records</t>
+  </si>
+  <si>
+    <t>Step 1: SAP Dashboard (Single URL)</t>
+  </si>
+  <si>
+    <t>Step 2: SAP Page</t>
+  </si>
+  <si>
+    <t>Step 3: Prepopulate survey</t>
+  </si>
+  <si>
+    <t>Step 4 : Template Selection Page</t>
+  </si>
+  <si>
+    <t>DMX Manual readings</t>
+  </si>
+  <si>
+    <t>1/~/2/~/3</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC32</t>
+  </si>
+  <si>
+    <t>DNT - Automation DMX Reading - Create New</t>
+  </si>
+  <si>
+    <t>Email Manager Tab wizard</t>
+  </si>
+  <si>
+    <t>Step 1: DM Page-Email Manager Tab</t>
+  </si>
+  <si>
+    <t>Step 2: Select an Email Template (Create New)</t>
+  </si>
+  <si>
+    <t>Step 3: Save the Template</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC33</t>
+  </si>
+  <si>
+    <t>Delete a Template Grid View</t>
+  </si>
+  <si>
+    <t>Step 1: Delete a Template Grid View</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC34</t>
+  </si>
+  <si>
+    <t>Delete a Template List View</t>
+  </si>
+  <si>
+    <t>Step 1: Delete a Template List View</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC35</t>
+  </si>
+  <si>
+    <t>Copy a Template Grid View</t>
+  </si>
+  <si>
+    <t>Step 1: Copy a Template Grid View</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC36</t>
+  </si>
+  <si>
+    <t>Copy a Template List View</t>
+  </si>
+  <si>
+    <t>Step 1: Copy a Template List View</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC37</t>
+  </si>
+  <si>
+    <t>Preview a Template Grid View</t>
+  </si>
+  <si>
+    <t>Step 1: Preview a Template Grid View</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC38</t>
+  </si>
+  <si>
+    <t>Preview a Template List View</t>
+  </si>
+  <si>
+    <t>Step 1: Preview a Template List View</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC39</t>
+  </si>
+  <si>
+    <t>Track survey Search 1 user</t>
+  </si>
+  <si>
+    <t>Step 1: Track survey page load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 2: Search record 1 </t>
+  </si>
+  <si>
+    <t>Step 3: Search record 2</t>
+  </si>
+  <si>
+    <t>channel</t>
+  </si>
+  <si>
+    <t>Single Use Link</t>
+  </si>
+  <si>
+    <t>searchRec1</t>
+  </si>
+  <si>
+    <t>searchRec2</t>
+  </si>
+  <si>
+    <t>kabirtest1@bluwberry.com291</t>
+  </si>
+  <si>
+    <t>kabirtest1@bluwberry.com292</t>
+  </si>
+  <si>
+    <t>textBox1</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC40</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Track survey Delete 100 records per page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 1: Track survey Page Deletion </t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC41</t>
+  </si>
+  <si>
+    <t>DNT- Automation DMX 999 list.xls</t>
+  </si>
+  <si>
+    <t>dateFormat</t>
+  </si>
+  <si>
+    <t>dd/mm/yyyy</t>
+  </si>
+  <si>
+    <t>Step 1: Schedule 999 records (By File)</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC42</t>
+  </si>
+  <si>
+    <t>Schedule 999 records (By List)</t>
+  </si>
+  <si>
+    <t>Step 1: Schedule 999 records (By List)</t>
+  </si>
+  <si>
+    <t>DNT- Automation DMX 999 list</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC43</t>
+  </si>
+  <si>
+    <t>Schedule 999 records (By File)</t>
+  </si>
+  <si>
+    <t>Schedule 999 records (Type Manually)</t>
+  </si>
+  <si>
+    <t>Step 1: Schedule 999 records (Type Manually)</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC44</t>
+  </si>
+  <si>
+    <t>Reminder Wizard (999 Invites in Surveys)</t>
+  </si>
+  <si>
+    <t>Step 1: Send/Schedule Reminder to all (Reminder Page)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 2: Select Reminder Message </t>
+  </si>
+  <si>
+    <t>Step 4 : Reminders Send/Schedule ALL (999 reminders)</t>
+  </si>
+  <si>
+    <t>DMX Manual Readings (999 Invites)</t>
+  </si>
+  <si>
+    <t>Step 3: Schedule Reminders</t>
+  </si>
+  <si>
+    <t>Step 6: Reminders ScheduledSelected (100) (diff pages 25 Email from Each page)</t>
+  </si>
+  <si>
+    <t>Step 5: Reminders Scheduled Selected (100) (Total 999 reminders)</t>
+  </si>
+  <si>
+    <t>Cancel reminders(1000)</t>
+  </si>
+  <si>
+    <t>DMX Manual Readings - Cancel 1000 Reminders</t>
+  </si>
+  <si>
+    <t>Step 1: Cancel 1000 Reminders</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC46</t>
+  </si>
+  <si>
+    <t>Publish on Facebook</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC47</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC48</t>
+  </si>
+  <si>
+    <t>Publish on Twiiter</t>
+  </si>
+  <si>
+    <t>Publish on LinkedIn</t>
+  </si>
+  <si>
+    <t>Step 1: Facebook Post Preview</t>
+  </si>
+  <si>
+    <t>Step 2: Publish on Facebook</t>
+  </si>
+  <si>
+    <t>Step 1: Twiiter Post Preview</t>
+  </si>
+  <si>
+    <t>Step 2: Publish on Twitter</t>
+  </si>
+  <si>
+    <t>Step 1: LinkedIn Post Preview</t>
+  </si>
+  <si>
+    <t>Step 2: Publish on LinkedIn</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC49</t>
+  </si>
+  <si>
+    <t>Send SMS Invite wizard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 1: Enter Mobile Numbers </t>
+  </si>
+  <si>
+    <t>Step 2: Pre-Populate Survey</t>
+  </si>
+  <si>
+    <t>Step 3: Prepop mismatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 4: Customize SMS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 5: Preview SMS </t>
+  </si>
+  <si>
+    <t>Step 6: Send/Schedule Invitations</t>
+  </si>
+  <si>
+    <t>SMS invitation numbers.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Template -21-Sep-2021 23:12:10 not present on page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Template -21-Sep-2021 23:52:50 not present on page.</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC45</t>
+  </si>
+  <si>
+    <t>I am proud to work at my school/~/Teaching gives me a feeling of accomplishment/~/Overall, I am satisfied with teaching/~/My current teaching duties are interesting/~/I am motivated to contribute more than what is expected of me at this school/~/I am not planning on leaving this school/~/I would feel comfortable referring a good friend to teach at this school/~/Overall, I enjoy working for this school’s principal</t>
+  </si>
+  <si>
+    <t>The school administrators make good decisions for the school overall/~/I enjoy the relationships I have with the school administrators/~/The classrooms where I teach are physically comfortable/~/My physical safety is protected at school/~/The school policies meet my needs as a teacher/~/The school supplies all the resources that I need to effectively teach my students/~/I fill a necessary role in the learning and growth of my students/~/I am a positive influence on my students</t>
   </si>
 </sst>
 </file>
@@ -633,7 +1098,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -659,6 +1124,7 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -672,6 +1138,22 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
@@ -715,7 +1197,7 @@
       <color indexed="12"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -730,6 +1212,16 @@
     </fill>
     <fill>
       <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="13"/>
       </patternFill>
     </fill>
@@ -840,7 +1332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -852,17 +1344,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1145,10 +1643,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,9 +1677,21 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{7C606FED-5AEC-4CC5-85C8-17130D54BD9E}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{DBA1180E-C10C-4824-B15F-688B2B07F360}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1232,10 +1742,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,24 +1798,41 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{59B4C049-04B3-4447-9A04-941BCA3EDEAB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B22B77-F9A0-48CA-B95A-663324812831}">
-  <dimension ref="A1:AS25"/>
+  <dimension ref="A1:BE50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
@@ -1315,10 +1842,10 @@
     <col min="8" max="8" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="11" max="44" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="11" max="56" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -1377,13 +1904,13 @@
         <v>51</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="W1" s="3" t="s">
         <v>59</v>
@@ -1437,25 +1964,61 @@
         <v>140</v>
       </c>
       <c r="AN1" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="AO1" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="AP1" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="AR1" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="AS1" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="AT1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="AU1" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="AV1" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="AW1" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="AX1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="AY1" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="AZ1" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="BA1" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="BB1" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="BC1" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="BD1" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="BE1" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -1479,10 +2042,12 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="5"/>
+      <c r="K2" s="5" t="s">
+        <v>218</v>
+      </c>
       <c r="L2" s="5" t="s">
         <v>47</v>
       </c>
@@ -1532,9 +2097,21 @@
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1"/>
       <c r="AR2" s="1"/>
-      <c r="AS2" s="4"/>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1"/>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" s="1"/>
+      <c r="BA2" s="1"/>
+      <c r="BB2" s="1"/>
+      <c r="BC2" s="1"/>
+      <c r="BD2" s="1"/>
+      <c r="BE2" s="4"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -1558,7 +2135,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="14" t="s">
         <v>27</v>
       </c>
       <c r="K3" s="5"/>
@@ -1609,9 +2186,21 @@
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
       <c r="AR3" s="1"/>
-      <c r="AS3" s="4"/>
+      <c r="AS3" s="1"/>
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
+      <c r="AW3" s="1"/>
+      <c r="AX3" s="1"/>
+      <c r="AY3" s="1"/>
+      <c r="AZ3" s="1"/>
+      <c r="BA3" s="1"/>
+      <c r="BB3" s="1"/>
+      <c r="BC3" s="1"/>
+      <c r="BD3" s="1"/>
+      <c r="BE3" s="4"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -1635,7 +2224,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="14" t="s">
         <v>27</v>
       </c>
       <c r="K4" s="5"/>
@@ -1686,9 +2275,21 @@
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
       <c r="AR4" s="1"/>
-      <c r="AS4" s="4"/>
+      <c r="AS4" s="1"/>
+      <c r="AT4" s="1"/>
+      <c r="AU4" s="1"/>
+      <c r="AV4" s="1"/>
+      <c r="AW4" s="1"/>
+      <c r="AX4" s="1"/>
+      <c r="AY4" s="1"/>
+      <c r="AZ4" s="1"/>
+      <c r="BA4" s="1"/>
+      <c r="BB4" s="1"/>
+      <c r="BC4" s="1"/>
+      <c r="BD4" s="1"/>
+      <c r="BE4" s="4"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -1712,7 +2313,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="14" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="5"/>
@@ -1763,14 +2364,26 @@
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
       <c r="AR5" s="1"/>
-      <c r="AS5" s="4"/>
+      <c r="AS5" s="1"/>
+      <c r="AT5" s="1"/>
+      <c r="AU5" s="1"/>
+      <c r="AV5" s="1"/>
+      <c r="AW5" s="1"/>
+      <c r="AX5" s="1"/>
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1"/>
+      <c r="BA5" s="1"/>
+      <c r="BB5" s="1"/>
+      <c r="BC5" s="1"/>
+      <c r="BD5" s="1"/>
+      <c r="BE5" s="4"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -1789,8 +2402,8 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="10" t="s">
-        <v>27</v>
+      <c r="J6" s="19" t="s">
+        <v>255</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5" t="s">
@@ -1856,9 +2469,21 @@
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>
       <c r="AR6" s="1"/>
-      <c r="AS6" s="4"/>
+      <c r="AS6" s="1"/>
+      <c r="AT6" s="1"/>
+      <c r="AU6" s="1"/>
+      <c r="AV6" s="1"/>
+      <c r="AW6" s="1"/>
+      <c r="AX6" s="1"/>
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1"/>
+      <c r="BA6" s="1"/>
+      <c r="BB6" s="1"/>
+      <c r="BC6" s="1"/>
+      <c r="BD6" s="1"/>
+      <c r="BE6" s="4"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>72</v>
       </c>
@@ -1882,7 +2507,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="6"/>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="14" t="s">
         <v>27</v>
       </c>
       <c r="K7" s="5"/>
@@ -1949,14 +2574,26 @@
       <c r="AP7" s="1"/>
       <c r="AQ7" s="1"/>
       <c r="AR7" s="1"/>
-      <c r="AS7" s="4"/>
+      <c r="AS7" s="1"/>
+      <c r="AT7" s="1"/>
+      <c r="AU7" s="1"/>
+      <c r="AV7" s="1"/>
+      <c r="AW7" s="1"/>
+      <c r="AX7" s="1"/>
+      <c r="AY7" s="1"/>
+      <c r="AZ7" s="1"/>
+      <c r="BA7" s="1"/>
+      <c r="BB7" s="1"/>
+      <c r="BC7" s="1"/>
+      <c r="BD7" s="1"/>
+      <c r="BE7" s="4"/>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -1975,8 +2612,8 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="10" t="s">
-        <v>27</v>
+      <c r="J8" s="20" t="s">
+        <v>255</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5" t="s">
@@ -2028,9 +2665,21 @@
       <c r="AP8" s="1"/>
       <c r="AQ8" s="1"/>
       <c r="AR8" s="1"/>
-      <c r="AS8" s="4"/>
+      <c r="AS8" s="1"/>
+      <c r="AT8" s="1"/>
+      <c r="AU8" s="1"/>
+      <c r="AV8" s="1"/>
+      <c r="AW8" s="1"/>
+      <c r="AX8" s="1"/>
+      <c r="AY8" s="1"/>
+      <c r="AZ8" s="1"/>
+      <c r="BA8" s="1"/>
+      <c r="BB8" s="1"/>
+      <c r="BC8" s="1"/>
+      <c r="BD8" s="1"/>
+      <c r="BE8" s="4"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>84</v>
       </c>
@@ -2054,7 +2703,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="14" t="s">
         <v>27</v>
       </c>
       <c r="K9" s="5"/>
@@ -2109,9 +2758,21 @@
       <c r="AP9" s="1"/>
       <c r="AQ9" s="1"/>
       <c r="AR9" s="1"/>
-      <c r="AS9" s="4"/>
+      <c r="AS9" s="1"/>
+      <c r="AT9" s="1"/>
+      <c r="AU9" s="1"/>
+      <c r="AV9" s="1"/>
+      <c r="AW9" s="1"/>
+      <c r="AX9" s="1"/>
+      <c r="AY9" s="1"/>
+      <c r="AZ9" s="1"/>
+      <c r="BA9" s="1"/>
+      <c r="BB9" s="1"/>
+      <c r="BC9" s="1"/>
+      <c r="BD9" s="1"/>
+      <c r="BE9" s="4"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>89</v>
       </c>
@@ -2135,7 +2796,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="14" t="s">
         <v>27</v>
       </c>
       <c r="K10" s="5"/>
@@ -2190,9 +2851,21 @@
       <c r="AP10" s="1"/>
       <c r="AQ10" s="1"/>
       <c r="AR10" s="1"/>
-      <c r="AS10" s="4"/>
+      <c r="AS10" s="1"/>
+      <c r="AT10" s="1"/>
+      <c r="AU10" s="1"/>
+      <c r="AV10" s="1"/>
+      <c r="AW10" s="1"/>
+      <c r="AX10" s="1"/>
+      <c r="AY10" s="1"/>
+      <c r="AZ10" s="1"/>
+      <c r="BA10" s="1"/>
+      <c r="BB10" s="1"/>
+      <c r="BC10" s="1"/>
+      <c r="BD10" s="1"/>
+      <c r="BE10" s="4"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>92</v>
       </c>
@@ -2216,7 +2889,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="14" t="s">
         <v>27</v>
       </c>
       <c r="K11" s="5"/>
@@ -2271,9 +2944,21 @@
       <c r="AP11" s="1"/>
       <c r="AQ11" s="1"/>
       <c r="AR11" s="1"/>
-      <c r="AS11" s="4"/>
+      <c r="AS11" s="1"/>
+      <c r="AT11" s="1"/>
+      <c r="AU11" s="1"/>
+      <c r="AV11" s="1"/>
+      <c r="AW11" s="1"/>
+      <c r="AX11" s="1"/>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="1"/>
+      <c r="BA11" s="1"/>
+      <c r="BB11" s="1"/>
+      <c r="BC11" s="1"/>
+      <c r="BD11" s="1"/>
+      <c r="BE11" s="4"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>95</v>
       </c>
@@ -2297,7 +2982,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="14" t="s">
         <v>27</v>
       </c>
       <c r="K12" s="5"/>
@@ -2352,9 +3037,21 @@
       <c r="AP12" s="1"/>
       <c r="AQ12" s="1"/>
       <c r="AR12" s="1"/>
-      <c r="AS12" s="4"/>
+      <c r="AS12" s="1"/>
+      <c r="AT12" s="1"/>
+      <c r="AU12" s="1"/>
+      <c r="AV12" s="1"/>
+      <c r="AW12" s="1"/>
+      <c r="AX12" s="1"/>
+      <c r="AY12" s="1"/>
+      <c r="AZ12" s="1"/>
+      <c r="BA12" s="1"/>
+      <c r="BB12" s="1"/>
+      <c r="BC12" s="1"/>
+      <c r="BD12" s="1"/>
+      <c r="BE12" s="4"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>104</v>
       </c>
@@ -2378,7 +3075,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="14" t="s">
         <v>27</v>
       </c>
       <c r="K13" s="5"/>
@@ -2435,9 +3132,21 @@
       <c r="AP13" s="7"/>
       <c r="AQ13" s="7"/>
       <c r="AR13" s="7"/>
-      <c r="AS13" s="4"/>
+      <c r="AS13" s="7"/>
+      <c r="AT13" s="7"/>
+      <c r="AU13" s="7"/>
+      <c r="AV13" s="7"/>
+      <c r="AW13" s="7"/>
+      <c r="AX13" s="7"/>
+      <c r="AY13" s="7"/>
+      <c r="AZ13" s="7"/>
+      <c r="BA13" s="7"/>
+      <c r="BB13" s="7"/>
+      <c r="BC13" s="7"/>
+      <c r="BD13" s="7"/>
+      <c r="BE13" s="4"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>107</v>
       </c>
@@ -2461,7 +3170,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="14" t="s">
         <v>27</v>
       </c>
       <c r="K14" s="5"/>
@@ -2518,9 +3227,21 @@
       <c r="AP14" s="8"/>
       <c r="AQ14" s="8"/>
       <c r="AR14" s="8"/>
-      <c r="AS14" s="4"/>
+      <c r="AS14" s="8"/>
+      <c r="AT14" s="8"/>
+      <c r="AU14" s="8"/>
+      <c r="AV14" s="8"/>
+      <c r="AW14" s="8"/>
+      <c r="AX14" s="8"/>
+      <c r="AY14" s="8"/>
+      <c r="AZ14" s="8"/>
+      <c r="BA14" s="8"/>
+      <c r="BB14" s="8"/>
+      <c r="BC14" s="8"/>
+      <c r="BD14" s="8"/>
+      <c r="BE14" s="4"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>118</v>
       </c>
@@ -2544,7 +3265,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="10" t="s">
+      <c r="J15" s="14" t="s">
         <v>27</v>
       </c>
       <c r="K15" s="5"/>
@@ -2595,9 +3316,21 @@
       <c r="AP15" s="8"/>
       <c r="AQ15" s="8"/>
       <c r="AR15" s="8"/>
-      <c r="AS15" s="4"/>
+      <c r="AS15" s="8"/>
+      <c r="AT15" s="8"/>
+      <c r="AU15" s="8"/>
+      <c r="AV15" s="8"/>
+      <c r="AW15" s="8"/>
+      <c r="AX15" s="8"/>
+      <c r="AY15" s="8"/>
+      <c r="AZ15" s="8"/>
+      <c r="BA15" s="8"/>
+      <c r="BB15" s="8"/>
+      <c r="BC15" s="8"/>
+      <c r="BD15" s="8"/>
+      <c r="BE15" s="4"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>121</v>
       </c>
@@ -2621,7 +3354,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="14" t="s">
         <v>27</v>
       </c>
       <c r="K16" s="5"/>
@@ -2664,9 +3397,21 @@
       <c r="AP16" s="8"/>
       <c r="AQ16" s="8"/>
       <c r="AR16" s="8"/>
-      <c r="AS16" s="4"/>
+      <c r="AS16" s="8"/>
+      <c r="AT16" s="8"/>
+      <c r="AU16" s="8"/>
+      <c r="AV16" s="8"/>
+      <c r="AW16" s="8"/>
+      <c r="AX16" s="8"/>
+      <c r="AY16" s="8"/>
+      <c r="AZ16" s="8"/>
+      <c r="BA16" s="8"/>
+      <c r="BB16" s="8"/>
+      <c r="BC16" s="8"/>
+      <c r="BD16" s="8"/>
+      <c r="BE16" s="4"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>123</v>
       </c>
@@ -2690,7 +3435,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="14" t="s">
         <v>27</v>
       </c>
       <c r="K17" s="5"/>
@@ -2743,9 +3488,21 @@
       <c r="AP17" s="8"/>
       <c r="AQ17" s="8"/>
       <c r="AR17" s="8"/>
-      <c r="AS17" s="4"/>
+      <c r="AS17" s="8"/>
+      <c r="AT17" s="8"/>
+      <c r="AU17" s="8"/>
+      <c r="AV17" s="8"/>
+      <c r="AW17" s="8"/>
+      <c r="AX17" s="8"/>
+      <c r="AY17" s="8"/>
+      <c r="AZ17" s="8"/>
+      <c r="BA17" s="8"/>
+      <c r="BB17" s="8"/>
+      <c r="BC17" s="8"/>
+      <c r="BD17" s="8"/>
+      <c r="BE17" s="4"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>128</v>
       </c>
@@ -2769,7 +3526,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="14" t="s">
         <v>27</v>
       </c>
       <c r="K18" s="5"/>
@@ -2824,9 +3581,21 @@
       <c r="AP18" s="8"/>
       <c r="AQ18" s="8"/>
       <c r="AR18" s="8"/>
-      <c r="AS18" s="4"/>
+      <c r="AS18" s="8"/>
+      <c r="AT18" s="8"/>
+      <c r="AU18" s="8"/>
+      <c r="AV18" s="8"/>
+      <c r="AW18" s="8"/>
+      <c r="AX18" s="8"/>
+      <c r="AY18" s="8"/>
+      <c r="AZ18" s="8"/>
+      <c r="BA18" s="8"/>
+      <c r="BB18" s="8"/>
+      <c r="BC18" s="8"/>
+      <c r="BD18" s="8"/>
+      <c r="BE18" s="4"/>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>131</v>
       </c>
@@ -2850,7 +3619,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="14" t="s">
         <v>27</v>
       </c>
       <c r="K19" s="5"/>
@@ -2911,14 +3680,26 @@
       <c r="AP19" s="1"/>
       <c r="AQ19" s="1"/>
       <c r="AR19" s="1"/>
-      <c r="AS19" s="4"/>
+      <c r="AS19" s="1"/>
+      <c r="AT19" s="1"/>
+      <c r="AU19" s="1"/>
+      <c r="AV19" s="1"/>
+      <c r="AW19" s="1"/>
+      <c r="AX19" s="1"/>
+      <c r="AY19" s="1"/>
+      <c r="AZ19" s="1"/>
+      <c r="BA19" s="1"/>
+      <c r="BB19" s="1"/>
+      <c r="BC19" s="1"/>
+      <c r="BD19" s="1"/>
+      <c r="BE19" s="4"/>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
@@ -2933,46 +3714,46 @@
         <v>43</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="9" t="s">
-        <v>141</v>
+      <c r="J20" s="22" t="s">
+        <v>255</v>
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="M20" s="5">
         <v>859</v>
       </c>
       <c r="N20" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q20" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="R20" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="S20" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="Q20" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="S20" s="1" t="s">
+      <c r="T20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="U20" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="T20" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="V20" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
@@ -2996,17 +3777,29 @@
       </c>
       <c r="AO20" s="1"/>
       <c r="AP20" s="1" t="s">
-        <v>146</v>
+        <v>354</v>
       </c>
       <c r="AQ20" s="1" t="s">
-        <v>147</v>
+        <v>355</v>
       </c>
       <c r="AR20" s="1"/>
-      <c r="AS20" s="4"/>
+      <c r="AS20" s="1"/>
+      <c r="AT20" s="1"/>
+      <c r="AU20" s="1"/>
+      <c r="AV20" s="1"/>
+      <c r="AW20" s="1"/>
+      <c r="AX20" s="1"/>
+      <c r="AY20" s="1"/>
+      <c r="AZ20" s="1"/>
+      <c r="BA20" s="1"/>
+      <c r="BB20" s="1"/>
+      <c r="BC20" s="1"/>
+      <c r="BD20" s="1"/>
+      <c r="BE20" s="4"/>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>26</v>
@@ -3024,12 +3817,12 @@
         <v>43</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="6"/>
-      <c r="J21" s="11" t="s">
-        <v>141</v>
+      <c r="J21" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5" t="s">
@@ -3039,16 +3832,16 @@
         <v>527</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>36</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="R21" s="1" t="s">
         <v>101</v>
@@ -3058,16 +3851,16 @@
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="Z21" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
@@ -3089,14 +3882,26 @@
       <c r="AP21" s="1"/>
       <c r="AQ21" s="1"/>
       <c r="AR21" s="1"/>
-      <c r="AS21" s="4"/>
+      <c r="AS21" s="1"/>
+      <c r="AT21" s="1"/>
+      <c r="AU21" s="1"/>
+      <c r="AV21" s="1"/>
+      <c r="AW21" s="1"/>
+      <c r="AX21" s="1"/>
+      <c r="AY21" s="1"/>
+      <c r="AZ21" s="1"/>
+      <c r="BA21" s="1"/>
+      <c r="BB21" s="1"/>
+      <c r="BC21" s="1"/>
+      <c r="BD21" s="1"/>
+      <c r="BE21" s="4"/>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
@@ -3111,12 +3916,12 @@
         <v>43</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="6"/>
-      <c r="J22" s="16" t="s">
-        <v>141</v>
+      <c r="J22" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5" t="s">
@@ -3126,16 +3931,16 @@
         <v>527</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>36</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="R22" s="1" t="s">
         <v>101</v>
@@ -3145,16 +3950,16 @@
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z22" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="X22" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="Y22" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="Z22" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
@@ -3176,11 +3981,23 @@
       <c r="AP22" s="1"/>
       <c r="AQ22" s="1"/>
       <c r="AR22" s="1"/>
-      <c r="AS22" s="4"/>
+      <c r="AS22" s="1"/>
+      <c r="AT22" s="1"/>
+      <c r="AU22" s="1"/>
+      <c r="AV22" s="1"/>
+      <c r="AW22" s="1"/>
+      <c r="AX22" s="1"/>
+      <c r="AY22" s="1"/>
+      <c r="AZ22" s="1"/>
+      <c r="BA22" s="1"/>
+      <c r="BB22" s="1"/>
+      <c r="BC22" s="1"/>
+      <c r="BD22" s="1"/>
+      <c r="BE22" s="4"/>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>26</v>
@@ -3198,12 +4015,12 @@
         <v>43</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="6"/>
-      <c r="J23" s="12" t="s">
-        <v>141</v>
+      <c r="J23" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5" t="s">
@@ -3213,13 +4030,13 @@
         <v>14</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>39</v>
@@ -3230,7 +4047,7 @@
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
       <c r="W23" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
@@ -3255,11 +4072,23 @@
       <c r="AP23" s="1"/>
       <c r="AQ23" s="1"/>
       <c r="AR23" s="1"/>
-      <c r="AS23" s="4"/>
+      <c r="AS23" s="1"/>
+      <c r="AT23" s="1"/>
+      <c r="AU23" s="1"/>
+      <c r="AV23" s="1"/>
+      <c r="AW23" s="1"/>
+      <c r="AX23" s="1"/>
+      <c r="AY23" s="1"/>
+      <c r="AZ23" s="1"/>
+      <c r="BA23" s="1"/>
+      <c r="BB23" s="1"/>
+      <c r="BC23" s="1"/>
+      <c r="BD23" s="1"/>
+      <c r="BE23" s="4"/>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>26</v>
@@ -3277,12 +4106,12 @@
         <v>43</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="6"/>
-      <c r="J24" s="13" t="s">
-        <v>141</v>
+      <c r="J24" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5" t="s">
@@ -3292,19 +4121,19 @@
         <v>527</v>
       </c>
       <c r="N24" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="R24" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="S24" s="1" t="s">
         <v>101</v>
@@ -3334,14 +4163,26 @@
       <c r="AP24" s="1"/>
       <c r="AQ24" s="1"/>
       <c r="AR24" s="1"/>
-      <c r="AS24" s="4"/>
+      <c r="AS24" s="1"/>
+      <c r="AT24" s="1"/>
+      <c r="AU24" s="1"/>
+      <c r="AV24" s="1"/>
+      <c r="AW24" s="1"/>
+      <c r="AX24" s="1"/>
+      <c r="AY24" s="1"/>
+      <c r="AZ24" s="1"/>
+      <c r="BA24" s="1"/>
+      <c r="BB24" s="1"/>
+      <c r="BC24" s="1"/>
+      <c r="BD24" s="1"/>
+      <c r="BE24" s="4"/>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>13</v>
@@ -3356,16 +4197,14 @@
         <v>43</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="6"/>
       <c r="J25" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>200</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="K25" s="5"/>
       <c r="L25" s="5" t="s">
         <v>47</v>
       </c>
@@ -3373,10 +4212,10 @@
         <v>527</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>57</v>
@@ -3385,13 +4224,13 @@
         <v>58</v>
       </c>
       <c r="R25" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="S25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="S25" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="T25" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="U25" s="1" t="s">
         <v>101</v>
@@ -3411,7 +4250,7 @@
       <c r="AH25" s="7"/>
       <c r="AI25" s="8"/>
       <c r="AJ25" s="8" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AK25" s="1"/>
       <c r="AL25" s="1"/>
@@ -3421,16 +4260,2255 @@
       <c r="AP25" s="1"/>
       <c r="AQ25" s="1"/>
       <c r="AR25" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="AS25" s="4"/>
+        <v>194</v>
+      </c>
+      <c r="AS25" s="2"/>
+      <c r="AT25" s="2"/>
+      <c r="AU25" s="2"/>
+      <c r="AV25" s="2"/>
+      <c r="AW25" s="2"/>
+      <c r="AX25" s="2"/>
+      <c r="AY25" s="2"/>
+      <c r="AZ25" s="2"/>
+      <c r="BA25" s="2"/>
+      <c r="BB25" s="2"/>
+      <c r="BC25" s="2"/>
+      <c r="BD25" s="2"/>
+      <c r="BE25" s="4"/>
+    </row>
+    <row r="26" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M26" s="5">
+        <v>890</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="1"/>
+      <c r="AF26" s="1"/>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="7"/>
+      <c r="AI26" s="8"/>
+      <c r="AJ26" s="8"/>
+      <c r="AK26" s="1"/>
+      <c r="AL26" s="1"/>
+      <c r="AM26" s="1"/>
+      <c r="AN26" s="1"/>
+      <c r="AO26" s="1"/>
+      <c r="AP26" s="1"/>
+      <c r="AQ26" s="1"/>
+      <c r="AR26" s="2"/>
+      <c r="AS26" s="2"/>
+      <c r="AT26" s="2"/>
+      <c r="AU26" s="2"/>
+      <c r="AV26" s="2"/>
+      <c r="AW26" s="2"/>
+      <c r="AX26" s="2"/>
+      <c r="AY26" s="2"/>
+      <c r="AZ26" s="2"/>
+      <c r="BA26" s="2"/>
+      <c r="BB26" s="2"/>
+      <c r="BC26" s="2"/>
+      <c r="BD26" s="2"/>
+      <c r="BE26" s="4"/>
+    </row>
+    <row r="27" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M27" s="5">
+        <v>890</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="W27" s="7"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="1"/>
+      <c r="AF27" s="1"/>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="7"/>
+      <c r="AI27" s="8"/>
+      <c r="AJ27" s="8"/>
+      <c r="AK27" s="1"/>
+      <c r="AL27" s="1"/>
+      <c r="AM27" s="1"/>
+      <c r="AN27" s="1"/>
+      <c r="AO27" s="1"/>
+      <c r="AP27" s="1"/>
+      <c r="AQ27" s="1"/>
+      <c r="AR27" s="2"/>
+      <c r="AS27" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="AT27" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="AU27" s="9"/>
+      <c r="AV27" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="AW27" s="8"/>
+      <c r="AX27" s="8"/>
+      <c r="AY27" s="8"/>
+      <c r="AZ27" s="8"/>
+      <c r="BA27" s="8"/>
+      <c r="BB27" s="8"/>
+      <c r="BC27" s="8"/>
+      <c r="BD27" s="8"/>
+      <c r="BE27" s="4"/>
+    </row>
+    <row r="28" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M28" s="5">
+        <v>890</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="U28" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="V28" s="1"/>
+      <c r="W28" s="7"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1"/>
+      <c r="AF28" s="1"/>
+      <c r="AG28" s="1"/>
+      <c r="AH28" s="7"/>
+      <c r="AI28" s="8"/>
+      <c r="AJ28" s="8"/>
+      <c r="AK28" s="1"/>
+      <c r="AL28" s="1"/>
+      <c r="AM28" s="1"/>
+      <c r="AN28" s="1"/>
+      <c r="AO28" s="1"/>
+      <c r="AP28" s="1"/>
+      <c r="AQ28" s="1"/>
+      <c r="AR28" s="2"/>
+      <c r="AS28" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="AT28" s="9"/>
+      <c r="AU28" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="AV28" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="AW28" s="8"/>
+      <c r="AX28" s="8"/>
+      <c r="AY28" s="8"/>
+      <c r="AZ28" s="8"/>
+      <c r="BA28" s="8"/>
+      <c r="BB28" s="8"/>
+      <c r="BC28" s="8"/>
+      <c r="BD28" s="8"/>
+      <c r="BE28" s="4"/>
+    </row>
+    <row r="29" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M29" s="5">
+        <v>890</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="V29" s="1"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="1"/>
+      <c r="AF29" s="1"/>
+      <c r="AG29" s="1"/>
+      <c r="AH29" s="7"/>
+      <c r="AI29" s="8"/>
+      <c r="AJ29" s="8"/>
+      <c r="AK29" s="1"/>
+      <c r="AL29" s="1"/>
+      <c r="AM29" s="1"/>
+      <c r="AN29" s="1"/>
+      <c r="AO29" s="1"/>
+      <c r="AP29" s="1"/>
+      <c r="AQ29" s="1"/>
+      <c r="AR29" s="2"/>
+      <c r="AS29" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="AT29" s="9"/>
+      <c r="AU29" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="AV29" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="AW29" s="8"/>
+      <c r="AX29" s="8"/>
+      <c r="AY29" s="8"/>
+      <c r="AZ29" s="8"/>
+      <c r="BA29" s="8"/>
+      <c r="BB29" s="8"/>
+      <c r="BC29" s="8"/>
+      <c r="BD29" s="8"/>
+      <c r="BE29" s="4"/>
+    </row>
+    <row r="30" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M30" s="5">
+        <v>890</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="1"/>
+      <c r="AF30" s="1"/>
+      <c r="AG30" s="1"/>
+      <c r="AH30" s="7"/>
+      <c r="AI30" s="8"/>
+      <c r="AJ30" s="8"/>
+      <c r="AK30" s="1"/>
+      <c r="AL30" s="1"/>
+      <c r="AM30" s="1"/>
+      <c r="AN30" s="1"/>
+      <c r="AO30" s="1"/>
+      <c r="AP30" s="1"/>
+      <c r="AQ30" s="1"/>
+      <c r="AR30" s="2"/>
+      <c r="AS30" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="AT30" s="9"/>
+      <c r="AU30" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="AV30" s="8"/>
+      <c r="AW30" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="AX30" s="8"/>
+      <c r="AY30" s="8"/>
+      <c r="AZ30" s="8"/>
+      <c r="BA30" s="8"/>
+      <c r="BB30" s="8"/>
+      <c r="BC30" s="8"/>
+      <c r="BD30" s="8"/>
+      <c r="BE30" s="4"/>
+    </row>
+    <row r="31" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M31" s="5">
+        <v>890</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="1"/>
+      <c r="AF31" s="1"/>
+      <c r="AG31" s="1"/>
+      <c r="AH31" s="7"/>
+      <c r="AI31" s="8"/>
+      <c r="AJ31" s="8"/>
+      <c r="AK31" s="1"/>
+      <c r="AL31" s="1"/>
+      <c r="AM31" s="1"/>
+      <c r="AN31" s="1"/>
+      <c r="AO31" s="1"/>
+      <c r="AP31" s="1"/>
+      <c r="AQ31" s="1"/>
+      <c r="AR31" s="2"/>
+      <c r="AS31" s="9"/>
+      <c r="AT31" s="9"/>
+      <c r="AU31" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="AV31" s="8"/>
+      <c r="AW31" s="8"/>
+      <c r="AX31" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="AY31" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="AZ31" s="8"/>
+      <c r="BA31" s="8"/>
+      <c r="BB31" s="8"/>
+      <c r="BC31" s="8"/>
+      <c r="BD31" s="8"/>
+      <c r="BE31" s="4"/>
+    </row>
+    <row r="32" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M32" s="5">
+        <v>890</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="1"/>
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="1"/>
+      <c r="AF32" s="1"/>
+      <c r="AG32" s="1"/>
+      <c r="AH32" s="7"/>
+      <c r="AI32" s="8"/>
+      <c r="AJ32" s="8"/>
+      <c r="AK32" s="1"/>
+      <c r="AL32" s="1"/>
+      <c r="AM32" s="1"/>
+      <c r="AN32" s="1"/>
+      <c r="AO32" s="1"/>
+      <c r="AP32" s="1"/>
+      <c r="AQ32" s="1"/>
+      <c r="AR32" s="2"/>
+      <c r="AS32" s="9"/>
+      <c r="AT32" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="AU32" s="9"/>
+      <c r="AV32" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="AW32" s="8"/>
+      <c r="AX32" s="8"/>
+      <c r="AY32" s="8"/>
+      <c r="AZ32" s="8"/>
+      <c r="BA32" s="8"/>
+      <c r="BB32" s="8"/>
+      <c r="BC32" s="8"/>
+      <c r="BD32" s="8"/>
+      <c r="BE32" s="4"/>
+    </row>
+    <row r="33" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M33" s="5">
+        <v>890</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="1"/>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="1"/>
+      <c r="AD33" s="1"/>
+      <c r="AE33" s="1"/>
+      <c r="AF33" s="1"/>
+      <c r="AG33" s="1"/>
+      <c r="AH33" s="7"/>
+      <c r="AI33" s="8"/>
+      <c r="AJ33" s="8"/>
+      <c r="AK33" s="1"/>
+      <c r="AL33" s="1"/>
+      <c r="AM33" s="1"/>
+      <c r="AN33" s="1"/>
+      <c r="AO33" s="1"/>
+      <c r="AP33" s="1"/>
+      <c r="AQ33" s="1"/>
+      <c r="AR33" s="2"/>
+      <c r="AS33" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="AT33" s="9"/>
+      <c r="AU33" s="9"/>
+      <c r="AV33" s="8"/>
+      <c r="AW33" s="8"/>
+      <c r="AX33" s="8"/>
+      <c r="AY33" s="8"/>
+      <c r="AZ33" s="8"/>
+      <c r="BA33" s="8"/>
+      <c r="BB33" s="8"/>
+      <c r="BC33" s="8"/>
+      <c r="BD33" s="8"/>
+      <c r="BE33" s="4"/>
+    </row>
+    <row r="34" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M34" s="5">
+        <v>890</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="7"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="1"/>
+      <c r="AB34" s="1"/>
+      <c r="AC34" s="1"/>
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="1"/>
+      <c r="AF34" s="1"/>
+      <c r="AG34" s="1"/>
+      <c r="AH34" s="7"/>
+      <c r="AI34" s="8"/>
+      <c r="AJ34" s="8"/>
+      <c r="AK34" s="1"/>
+      <c r="AL34" s="1"/>
+      <c r="AM34" s="1"/>
+      <c r="AN34" s="1"/>
+      <c r="AO34" s="1"/>
+      <c r="AP34" s="1"/>
+      <c r="AQ34" s="1"/>
+      <c r="AR34" s="2"/>
+      <c r="AS34" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="AT34" s="9"/>
+      <c r="AU34" s="9"/>
+      <c r="AV34" s="8"/>
+      <c r="AW34" s="8"/>
+      <c r="AX34" s="8"/>
+      <c r="AY34" s="8"/>
+      <c r="AZ34" s="8"/>
+      <c r="BA34" s="8"/>
+      <c r="BB34" s="8"/>
+      <c r="BC34" s="8"/>
+      <c r="BD34" s="8"/>
+      <c r="BE34" s="4"/>
+    </row>
+    <row r="35" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M35" s="5">
+        <v>890</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="1"/>
+      <c r="Y35" s="1"/>
+      <c r="Z35" s="1"/>
+      <c r="AA35" s="1"/>
+      <c r="AB35" s="1"/>
+      <c r="AC35" s="1"/>
+      <c r="AD35" s="1"/>
+      <c r="AE35" s="1"/>
+      <c r="AF35" s="1"/>
+      <c r="AG35" s="1"/>
+      <c r="AH35" s="7"/>
+      <c r="AI35" s="8"/>
+      <c r="AJ35" s="8"/>
+      <c r="AK35" s="1"/>
+      <c r="AL35" s="1"/>
+      <c r="AM35" s="1"/>
+      <c r="AN35" s="1"/>
+      <c r="AO35" s="1"/>
+      <c r="AP35" s="1"/>
+      <c r="AQ35" s="1"/>
+      <c r="AR35" s="2"/>
+      <c r="AS35" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="AT35" s="9"/>
+      <c r="AU35" s="9"/>
+      <c r="AV35" s="8"/>
+      <c r="AW35" s="8"/>
+      <c r="AX35" s="8"/>
+      <c r="AY35" s="8"/>
+      <c r="AZ35" s="8"/>
+      <c r="BA35" s="8"/>
+      <c r="BB35" s="8"/>
+      <c r="BC35" s="8"/>
+      <c r="BD35" s="8"/>
+      <c r="BE35" s="4"/>
+    </row>
+    <row r="36" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M36" s="5">
+        <v>890</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
+      <c r="AA36" s="1"/>
+      <c r="AB36" s="1"/>
+      <c r="AC36" s="1"/>
+      <c r="AD36" s="1"/>
+      <c r="AE36" s="1"/>
+      <c r="AF36" s="1"/>
+      <c r="AG36" s="1"/>
+      <c r="AH36" s="7"/>
+      <c r="AI36" s="8"/>
+      <c r="AJ36" s="8"/>
+      <c r="AK36" s="1"/>
+      <c r="AL36" s="1"/>
+      <c r="AM36" s="1"/>
+      <c r="AN36" s="1"/>
+      <c r="AO36" s="1"/>
+      <c r="AP36" s="1"/>
+      <c r="AQ36" s="1"/>
+      <c r="AR36" s="2"/>
+      <c r="AS36" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="AT36" s="9"/>
+      <c r="AU36" s="9"/>
+      <c r="AV36" s="8"/>
+      <c r="AW36" s="8"/>
+      <c r="AX36" s="8"/>
+      <c r="AY36" s="8"/>
+      <c r="AZ36" s="8"/>
+      <c r="BA36" s="8"/>
+      <c r="BB36" s="8"/>
+      <c r="BC36" s="8"/>
+      <c r="BD36" s="8"/>
+      <c r="BE36" s="4"/>
+    </row>
+    <row r="37" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M37" s="5">
+        <v>890</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="7"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1"/>
+      <c r="AA37" s="1"/>
+      <c r="AB37" s="1"/>
+      <c r="AC37" s="1"/>
+      <c r="AD37" s="1"/>
+      <c r="AE37" s="1"/>
+      <c r="AF37" s="1"/>
+      <c r="AG37" s="1"/>
+      <c r="AH37" s="7"/>
+      <c r="AI37" s="8"/>
+      <c r="AJ37" s="8"/>
+      <c r="AK37" s="1"/>
+      <c r="AL37" s="1"/>
+      <c r="AM37" s="1"/>
+      <c r="AN37" s="1"/>
+      <c r="AO37" s="1"/>
+      <c r="AP37" s="1"/>
+      <c r="AQ37" s="1"/>
+      <c r="AR37" s="2"/>
+      <c r="AS37" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="AT37" s="9"/>
+      <c r="AU37" s="9"/>
+      <c r="AV37" s="8"/>
+      <c r="AW37" s="8"/>
+      <c r="AX37" s="8"/>
+      <c r="AY37" s="8"/>
+      <c r="AZ37" s="8"/>
+      <c r="BA37" s="8"/>
+      <c r="BB37" s="8"/>
+      <c r="BC37" s="8"/>
+      <c r="BD37" s="8"/>
+      <c r="BE37" s="4"/>
+    </row>
+    <row r="38" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M38" s="5">
+        <v>890</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1"/>
+      <c r="AB38" s="1"/>
+      <c r="AC38" s="1"/>
+      <c r="AD38" s="1"/>
+      <c r="AE38" s="1"/>
+      <c r="AF38" s="1"/>
+      <c r="AG38" s="1"/>
+      <c r="AH38" s="7"/>
+      <c r="AI38" s="8"/>
+      <c r="AJ38" s="8"/>
+      <c r="AK38" s="1"/>
+      <c r="AL38" s="1"/>
+      <c r="AM38" s="1"/>
+      <c r="AN38" s="1"/>
+      <c r="AO38" s="1"/>
+      <c r="AP38" s="1"/>
+      <c r="AQ38" s="1"/>
+      <c r="AR38" s="2"/>
+      <c r="AS38" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="AT38" s="9"/>
+      <c r="AU38" s="9"/>
+      <c r="AV38" s="8"/>
+      <c r="AW38" s="8"/>
+      <c r="AX38" s="8"/>
+      <c r="AY38" s="8"/>
+      <c r="AZ38" s="8"/>
+      <c r="BA38" s="8"/>
+      <c r="BB38" s="8"/>
+      <c r="BC38" s="8"/>
+      <c r="BD38" s="8"/>
+      <c r="BE38" s="4"/>
+    </row>
+    <row r="39" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H39" s="1"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M39" s="5">
+        <v>890</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="7"/>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
+      <c r="Z39" s="1"/>
+      <c r="AA39" s="1"/>
+      <c r="AB39" s="1"/>
+      <c r="AC39" s="1"/>
+      <c r="AD39" s="1"/>
+      <c r="AE39" s="1"/>
+      <c r="AF39" s="1"/>
+      <c r="AG39" s="1"/>
+      <c r="AH39" s="7"/>
+      <c r="AI39" s="8"/>
+      <c r="AJ39" s="8"/>
+      <c r="AK39" s="1"/>
+      <c r="AL39" s="1"/>
+      <c r="AM39" s="1"/>
+      <c r="AN39" s="1"/>
+      <c r="AO39" s="1"/>
+      <c r="AP39" s="1"/>
+      <c r="AQ39" s="1"/>
+      <c r="AR39" s="2"/>
+      <c r="AS39" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="AT39" s="9"/>
+      <c r="AU39" s="9"/>
+      <c r="AV39" s="8"/>
+      <c r="AW39" s="8"/>
+      <c r="AX39" s="8"/>
+      <c r="AY39" s="8"/>
+      <c r="AZ39" s="8"/>
+      <c r="BA39" s="8"/>
+      <c r="BB39" s="8"/>
+      <c r="BC39" s="8"/>
+      <c r="BD39" s="8"/>
+      <c r="BE39" s="4"/>
+    </row>
+    <row r="40" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H40" s="1"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M40" s="5">
+        <v>890</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="7"/>
+      <c r="X40" s="1"/>
+      <c r="Y40" s="1"/>
+      <c r="Z40" s="1"/>
+      <c r="AA40" s="1"/>
+      <c r="AB40" s="1"/>
+      <c r="AC40" s="1"/>
+      <c r="AD40" s="1"/>
+      <c r="AE40" s="1"/>
+      <c r="AF40" s="1"/>
+      <c r="AG40" s="1"/>
+      <c r="AH40" s="7"/>
+      <c r="AI40" s="8"/>
+      <c r="AJ40" s="8"/>
+      <c r="AK40" s="1"/>
+      <c r="AL40" s="1"/>
+      <c r="AM40" s="1"/>
+      <c r="AN40" s="1"/>
+      <c r="AO40" s="1"/>
+      <c r="AP40" s="1"/>
+      <c r="AQ40" s="1"/>
+      <c r="AR40" s="2"/>
+      <c r="AS40" s="9"/>
+      <c r="AT40" s="9"/>
+      <c r="AU40" s="9"/>
+      <c r="AV40" s="8"/>
+      <c r="AW40" s="8"/>
+      <c r="AX40" s="8"/>
+      <c r="AY40" s="8"/>
+      <c r="AZ40" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="BA40" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="BB40" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="BC40" s="11"/>
+      <c r="BD40" s="11"/>
+      <c r="BE40" s="4"/>
+    </row>
+    <row r="41" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="H41" s="1"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M41" s="5">
+        <v>890</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="7"/>
+      <c r="X41" s="1"/>
+      <c r="Y41" s="1"/>
+      <c r="Z41" s="1"/>
+      <c r="AA41" s="1"/>
+      <c r="AB41" s="1"/>
+      <c r="AC41" s="1"/>
+      <c r="AD41" s="1"/>
+      <c r="AE41" s="1"/>
+      <c r="AF41" s="1"/>
+      <c r="AG41" s="1"/>
+      <c r="AH41" s="7"/>
+      <c r="AI41" s="8"/>
+      <c r="AJ41" s="8"/>
+      <c r="AK41" s="1"/>
+      <c r="AL41" s="1"/>
+      <c r="AM41" s="1"/>
+      <c r="AN41" s="1"/>
+      <c r="AO41" s="1"/>
+      <c r="AP41" s="1"/>
+      <c r="AQ41" s="1"/>
+      <c r="AR41" s="2"/>
+      <c r="AS41" s="9"/>
+      <c r="AT41" s="9"/>
+      <c r="AU41" s="9"/>
+      <c r="AV41" s="8"/>
+      <c r="AW41" s="8"/>
+      <c r="AX41" s="8"/>
+      <c r="AY41" s="8"/>
+      <c r="AZ41" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="BA41" s="10"/>
+      <c r="BB41" s="10"/>
+      <c r="BC41" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="BD41" s="11"/>
+      <c r="BE41" s="4"/>
+    </row>
+    <row r="42" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="H42" s="1"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M42" s="5">
+        <v>890</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="7"/>
+      <c r="X42" s="1"/>
+      <c r="Y42" s="1"/>
+      <c r="Z42" s="1"/>
+      <c r="AA42" s="1"/>
+      <c r="AB42" s="1"/>
+      <c r="AC42" s="1"/>
+      <c r="AD42" s="1"/>
+      <c r="AE42" s="1"/>
+      <c r="AF42" s="1"/>
+      <c r="AG42" s="1"/>
+      <c r="AH42" s="7"/>
+      <c r="AI42" s="8"/>
+      <c r="AJ42" s="8"/>
+      <c r="AK42" s="1"/>
+      <c r="AL42" s="1"/>
+      <c r="AM42" s="1"/>
+      <c r="AN42" s="1"/>
+      <c r="AO42" s="1"/>
+      <c r="AP42" s="1"/>
+      <c r="AQ42" s="1"/>
+      <c r="AR42" s="2"/>
+      <c r="AS42" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="AT42" s="9"/>
+      <c r="AU42" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="AV42" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="AW42" s="8"/>
+      <c r="AX42" s="8"/>
+      <c r="AY42" s="8"/>
+      <c r="AZ42" s="8"/>
+      <c r="BA42" s="10"/>
+      <c r="BB42" s="10"/>
+      <c r="BC42" s="11"/>
+      <c r="BD42" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="BE42" s="4"/>
+    </row>
+    <row r="43" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H43" s="1"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M43" s="5">
+        <v>890</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="7"/>
+      <c r="X43" s="1"/>
+      <c r="Y43" s="1"/>
+      <c r="Z43" s="1"/>
+      <c r="AA43" s="1"/>
+      <c r="AB43" s="1"/>
+      <c r="AC43" s="1"/>
+      <c r="AD43" s="1"/>
+      <c r="AE43" s="1"/>
+      <c r="AF43" s="1"/>
+      <c r="AG43" s="1"/>
+      <c r="AH43" s="7"/>
+      <c r="AI43" s="8"/>
+      <c r="AJ43" s="8"/>
+      <c r="AK43" s="1"/>
+      <c r="AL43" s="1"/>
+      <c r="AM43" s="1"/>
+      <c r="AN43" s="1"/>
+      <c r="AO43" s="1"/>
+      <c r="AP43" s="1"/>
+      <c r="AQ43" s="1"/>
+      <c r="AR43" s="2"/>
+      <c r="AS43" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="AT43" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="AU43" s="9"/>
+      <c r="AV43" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="AW43" s="8"/>
+      <c r="AX43" s="8"/>
+      <c r="AY43" s="8"/>
+      <c r="AZ43" s="8"/>
+      <c r="BA43" s="10"/>
+      <c r="BB43" s="10"/>
+      <c r="BC43" s="11"/>
+      <c r="BD43" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="BE43" s="4"/>
+    </row>
+    <row r="44" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="H44" s="1"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M44" s="5">
+        <v>890</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="7"/>
+      <c r="X44" s="1"/>
+      <c r="Y44" s="1"/>
+      <c r="Z44" s="1"/>
+      <c r="AA44" s="1"/>
+      <c r="AB44" s="1"/>
+      <c r="AC44" s="1"/>
+      <c r="AD44" s="1"/>
+      <c r="AE44" s="1"/>
+      <c r="AF44" s="1"/>
+      <c r="AG44" s="1"/>
+      <c r="AH44" s="7"/>
+      <c r="AI44" s="8"/>
+      <c r="AJ44" s="8"/>
+      <c r="AK44" s="1"/>
+      <c r="AL44" s="1"/>
+      <c r="AM44" s="1"/>
+      <c r="AN44" s="1"/>
+      <c r="AO44" s="1"/>
+      <c r="AP44" s="1"/>
+      <c r="AQ44" s="1"/>
+      <c r="AR44" s="2"/>
+      <c r="AS44" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="AT44" s="9"/>
+      <c r="AU44" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="AV44" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="AW44" s="8"/>
+      <c r="AX44" s="8"/>
+      <c r="AY44" s="8"/>
+      <c r="AZ44" s="8"/>
+      <c r="BA44" s="10"/>
+      <c r="BB44" s="10"/>
+      <c r="BC44" s="11"/>
+      <c r="BD44" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="BE44" s="4"/>
+    </row>
+    <row r="45" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="H45" s="1"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K45" s="5"/>
+      <c r="L45" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="M45" s="5">
+        <v>1288</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q45" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="S45" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="7"/>
+      <c r="X45" s="1"/>
+      <c r="Y45" s="1"/>
+      <c r="Z45" s="1"/>
+      <c r="AA45" s="1"/>
+      <c r="AB45" s="1"/>
+      <c r="AC45" s="1"/>
+      <c r="AD45" s="1"/>
+      <c r="AE45" s="1"/>
+      <c r="AF45" s="1"/>
+      <c r="AG45" s="1"/>
+      <c r="AH45" s="7"/>
+      <c r="AI45" s="8"/>
+      <c r="AJ45" s="8"/>
+      <c r="AK45" s="1"/>
+      <c r="AL45" s="1"/>
+      <c r="AM45" s="1"/>
+      <c r="AN45" s="1">
+        <v>25</v>
+      </c>
+      <c r="AO45" s="1"/>
+      <c r="AP45" s="1"/>
+      <c r="AQ45" s="1"/>
+      <c r="AR45" s="2"/>
+      <c r="AS45" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="AT45" s="9"/>
+      <c r="AU45" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="AV45" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="AW45" s="8"/>
+      <c r="AX45" s="8"/>
+      <c r="AY45" s="8"/>
+      <c r="AZ45" s="8"/>
+      <c r="BA45" s="10"/>
+      <c r="BB45" s="10"/>
+      <c r="BC45" s="11">
+        <v>4</v>
+      </c>
+      <c r="BD45" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="BE45" s="4"/>
+    </row>
+    <row r="46" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="H46" s="1"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="K46" s="5"/>
+      <c r="L46" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="M46" s="5">
+        <v>1311</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
+      <c r="W46" s="7"/>
+      <c r="X46" s="1"/>
+      <c r="Y46" s="1"/>
+      <c r="Z46" s="1"/>
+      <c r="AA46" s="1"/>
+      <c r="AB46" s="1"/>
+      <c r="AC46" s="1"/>
+      <c r="AD46" s="1"/>
+      <c r="AE46" s="1"/>
+      <c r="AF46" s="1"/>
+      <c r="AG46" s="1"/>
+      <c r="AH46" s="7"/>
+      <c r="AI46" s="8"/>
+      <c r="AJ46" s="8"/>
+      <c r="AK46" s="1"/>
+      <c r="AL46" s="1"/>
+      <c r="AM46" s="1"/>
+      <c r="AN46" s="1"/>
+      <c r="AO46" s="1"/>
+      <c r="AP46" s="1"/>
+      <c r="AQ46" s="1"/>
+      <c r="AR46" s="2"/>
+      <c r="AS46" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="AT46" s="9"/>
+      <c r="AU46" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="AV46" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="AW46" s="8"/>
+      <c r="AX46" s="8"/>
+      <c r="AY46" s="8"/>
+      <c r="AZ46" s="8"/>
+      <c r="BA46" s="10"/>
+      <c r="BB46" s="10"/>
+      <c r="BC46" s="11"/>
+      <c r="BD46" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="BE46" s="4"/>
+    </row>
+    <row r="47" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="H47" s="1"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M47" s="5">
+        <v>890</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="7"/>
+      <c r="X47" s="1"/>
+      <c r="Y47" s="1"/>
+      <c r="Z47" s="1"/>
+      <c r="AA47" s="1"/>
+      <c r="AB47" s="1"/>
+      <c r="AC47" s="1"/>
+      <c r="AD47" s="1"/>
+      <c r="AE47" s="1"/>
+      <c r="AF47" s="1"/>
+      <c r="AG47" s="1"/>
+      <c r="AH47" s="7"/>
+      <c r="AI47" s="8"/>
+      <c r="AJ47" s="8"/>
+      <c r="AK47" s="1"/>
+      <c r="AL47" s="1"/>
+      <c r="AM47" s="1"/>
+      <c r="AN47" s="1"/>
+      <c r="AO47" s="1"/>
+      <c r="AP47" s="1"/>
+      <c r="AQ47" s="1"/>
+      <c r="AR47" s="2"/>
+      <c r="AS47" s="9"/>
+      <c r="AT47" s="9"/>
+      <c r="AU47" s="9"/>
+      <c r="AV47" s="8"/>
+      <c r="AW47" s="8"/>
+      <c r="AX47" s="8"/>
+      <c r="AY47" s="8"/>
+      <c r="AZ47" s="8"/>
+      <c r="BA47" s="10"/>
+      <c r="BB47" s="10"/>
+      <c r="BC47" s="11"/>
+      <c r="BD47" s="11"/>
+      <c r="BE47" s="4"/>
+    </row>
+    <row r="48" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="H48" s="1"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M48" s="5">
+        <v>890</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="7"/>
+      <c r="X48" s="1"/>
+      <c r="Y48" s="1"/>
+      <c r="Z48" s="1"/>
+      <c r="AA48" s="1"/>
+      <c r="AB48" s="1"/>
+      <c r="AC48" s="1"/>
+      <c r="AD48" s="1"/>
+      <c r="AE48" s="1"/>
+      <c r="AF48" s="1"/>
+      <c r="AG48" s="1"/>
+      <c r="AH48" s="7"/>
+      <c r="AI48" s="8"/>
+      <c r="AJ48" s="8"/>
+      <c r="AK48" s="1"/>
+      <c r="AL48" s="1"/>
+      <c r="AM48" s="1"/>
+      <c r="AN48" s="1"/>
+      <c r="AO48" s="1"/>
+      <c r="AP48" s="1"/>
+      <c r="AQ48" s="1"/>
+      <c r="AR48" s="2"/>
+      <c r="AS48" s="9"/>
+      <c r="AT48" s="9"/>
+      <c r="AU48" s="9"/>
+      <c r="AV48" s="8"/>
+      <c r="AW48" s="8"/>
+      <c r="AX48" s="8"/>
+      <c r="AY48" s="8"/>
+      <c r="AZ48" s="8"/>
+      <c r="BA48" s="10"/>
+      <c r="BB48" s="10"/>
+      <c r="BC48" s="11"/>
+      <c r="BD48" s="11"/>
+      <c r="BE48" s="4"/>
+    </row>
+    <row r="49" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="H49" s="1"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M49" s="5">
+        <v>890</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+      <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+      <c r="W49" s="7"/>
+      <c r="X49" s="1"/>
+      <c r="Y49" s="1"/>
+      <c r="Z49" s="1"/>
+      <c r="AA49" s="1"/>
+      <c r="AB49" s="1"/>
+      <c r="AC49" s="1"/>
+      <c r="AD49" s="1"/>
+      <c r="AE49" s="1"/>
+      <c r="AF49" s="1"/>
+      <c r="AG49" s="1"/>
+      <c r="AH49" s="7"/>
+      <c r="AI49" s="8"/>
+      <c r="AJ49" s="8"/>
+      <c r="AK49" s="1"/>
+      <c r="AL49" s="1"/>
+      <c r="AM49" s="1"/>
+      <c r="AN49" s="1"/>
+      <c r="AO49" s="1"/>
+      <c r="AP49" s="1"/>
+      <c r="AQ49" s="1"/>
+      <c r="AR49" s="2"/>
+      <c r="AS49" s="9"/>
+      <c r="AT49" s="9"/>
+      <c r="AU49" s="9"/>
+      <c r="AV49" s="8"/>
+      <c r="AW49" s="8"/>
+      <c r="AX49" s="8"/>
+      <c r="AY49" s="8"/>
+      <c r="AZ49" s="8"/>
+      <c r="BA49" s="10"/>
+      <c r="BB49" s="10"/>
+      <c r="BC49" s="11"/>
+      <c r="BD49" s="11"/>
+      <c r="BE49" s="4"/>
+    </row>
+    <row r="50" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="H50" s="1"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="M50" s="5">
+        <v>890</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="Q50" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="R50" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="S50" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="T50" s="1"/>
+      <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
+      <c r="W50" s="7"/>
+      <c r="X50" s="1"/>
+      <c r="Y50" s="1"/>
+      <c r="Z50" s="1"/>
+      <c r="AA50" s="1"/>
+      <c r="AB50" s="1"/>
+      <c r="AC50" s="1"/>
+      <c r="AD50" s="1"/>
+      <c r="AE50" s="1"/>
+      <c r="AF50" s="1"/>
+      <c r="AG50" s="1"/>
+      <c r="AH50" s="7"/>
+      <c r="AI50" s="8"/>
+      <c r="AJ50" s="8"/>
+      <c r="AK50" s="1"/>
+      <c r="AL50" s="1"/>
+      <c r="AM50" s="1"/>
+      <c r="AN50" s="1"/>
+      <c r="AO50" s="1"/>
+      <c r="AP50" s="1"/>
+      <c r="AQ50" s="1"/>
+      <c r="AR50" s="2"/>
+      <c r="AS50" s="9"/>
+      <c r="AT50" s="9"/>
+      <c r="AU50" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="AV50" s="8"/>
+      <c r="AW50" s="8"/>
+      <c r="AX50" s="8"/>
+      <c r="AY50" s="8"/>
+      <c r="AZ50" s="8"/>
+      <c r="BA50" s="10"/>
+      <c r="BB50" s="10"/>
+      <c r="BC50" s="11"/>
+      <c r="BD50" s="11"/>
+      <c r="BE50" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="AR25" r:id="rId1" xr:uid="{FCAF826B-C13B-457E-A6AA-2797C89CE965}"/>
+    <hyperlink ref="BA40" r:id="rId2" xr:uid="{395D0E44-5176-44FC-A0E3-4406C6056A59}"/>
+    <hyperlink ref="BB40" r:id="rId3" xr:uid="{133777FB-04CC-435B-AF97-FFB564696B44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Response rate and Adv freq readings added for sogo, k12 and zarca.
</commit_message>
<xml_diff>
--- a/Engage/Engage-Performance/src/main/resources/excelfiles/Engage_PlatformReadings.xlsx
+++ b/Engage/Engage-Performance/src/main/resources/excelfiles/Engage_PlatformReadings.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F3861A-F49D-4FC8-A44D-90AEB0970390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BA1057-F6EF-44F8-B0A0-BCE9A4670454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="3045" windowWidth="15375" windowHeight="7875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="364">
   <si>
     <t>Environment</t>
   </si>
@@ -679,9 +679,6 @@
     <t>Step 6: Pre-Populate Survey</t>
   </si>
   <si>
-    <t xml:space="preserve"> Quick send button not present on page.</t>
-  </si>
-  <si>
     <t>Email Address/~/First Name/~/Last Name</t>
   </si>
   <si>
@@ -790,315 +787,341 @@
     <t>Email Address/~/First Name/~/Last Name/~/Company</t>
   </si>
   <si>
+    <t>Step 5: Delete Same List</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC31</t>
+  </si>
+  <si>
+    <t>Offline invites for 999  records</t>
+  </si>
+  <si>
+    <t>Step 1: SAP Dashboard (Single URL)</t>
+  </si>
+  <si>
+    <t>Step 2: SAP Page</t>
+  </si>
+  <si>
+    <t>Step 3: Prepopulate survey</t>
+  </si>
+  <si>
+    <t>Step 4 : Template Selection Page</t>
+  </si>
+  <si>
+    <t>DMX Manual readings</t>
+  </si>
+  <si>
+    <t>1/~/2/~/3</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC32</t>
+  </si>
+  <si>
+    <t>DNT - Automation DMX Reading - Create New</t>
+  </si>
+  <si>
+    <t>Email Manager Tab wizard</t>
+  </si>
+  <si>
+    <t>Step 1: DM Page-Email Manager Tab</t>
+  </si>
+  <si>
+    <t>Step 2: Select an Email Template (Create New)</t>
+  </si>
+  <si>
+    <t>Step 3: Save the Template</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC33</t>
+  </si>
+  <si>
+    <t>Delete a Template Grid View</t>
+  </si>
+  <si>
+    <t>Step 1: Delete a Template Grid View</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC34</t>
+  </si>
+  <si>
+    <t>Delete a Template List View</t>
+  </si>
+  <si>
+    <t>Step 1: Delete a Template List View</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC35</t>
+  </si>
+  <si>
+    <t>Copy a Template Grid View</t>
+  </si>
+  <si>
+    <t>Step 1: Copy a Template Grid View</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC36</t>
+  </si>
+  <si>
+    <t>Copy a Template List View</t>
+  </si>
+  <si>
+    <t>Step 1: Copy a Template List View</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC37</t>
+  </si>
+  <si>
+    <t>Preview a Template Grid View</t>
+  </si>
+  <si>
+    <t>Step 1: Preview a Template Grid View</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC38</t>
+  </si>
+  <si>
+    <t>Preview a Template List View</t>
+  </si>
+  <si>
+    <t>Step 1: Preview a Template List View</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC39</t>
+  </si>
+  <si>
+    <t>Track survey Search 1 user</t>
+  </si>
+  <si>
+    <t>Step 1: Track survey page load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 2: Search record 1 </t>
+  </si>
+  <si>
+    <t>Step 3: Search record 2</t>
+  </si>
+  <si>
+    <t>channel</t>
+  </si>
+  <si>
+    <t>Single Use Link</t>
+  </si>
+  <si>
+    <t>searchRec1</t>
+  </si>
+  <si>
+    <t>searchRec2</t>
+  </si>
+  <si>
+    <t>kabirtest1@bluwberry.com291</t>
+  </si>
+  <si>
+    <t>kabirtest1@bluwberry.com292</t>
+  </si>
+  <si>
+    <t>textBox1</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC40</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Track survey Delete 100 records per page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 1: Track survey Page Deletion </t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC41</t>
+  </si>
+  <si>
+    <t>DNT- Automation DMX 999 list.xls</t>
+  </si>
+  <si>
+    <t>dateFormat</t>
+  </si>
+  <si>
+    <t>dd/mm/yyyy</t>
+  </si>
+  <si>
+    <t>Step 1: Schedule 999 records (By File)</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC42</t>
+  </si>
+  <si>
+    <t>Schedule 999 records (By List)</t>
+  </si>
+  <si>
+    <t>Step 1: Schedule 999 records (By List)</t>
+  </si>
+  <si>
+    <t>DNT- Automation DMX 999 list</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC43</t>
+  </si>
+  <si>
+    <t>Schedule 999 records (By File)</t>
+  </si>
+  <si>
+    <t>Schedule 999 records (Type Manually)</t>
+  </si>
+  <si>
+    <t>Step 1: Schedule 999 records (Type Manually)</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC44</t>
+  </si>
+  <si>
+    <t>Reminder Wizard (999 Invites in Surveys)</t>
+  </si>
+  <si>
+    <t>Step 1: Send/Schedule Reminder to all (Reminder Page)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 2: Select Reminder Message </t>
+  </si>
+  <si>
+    <t>Step 4 : Reminders Send/Schedule ALL (999 reminders)</t>
+  </si>
+  <si>
+    <t>DMX Manual Readings (999 Invites)</t>
+  </si>
+  <si>
+    <t>Step 3: Schedule Reminders</t>
+  </si>
+  <si>
+    <t>Step 6: Reminders ScheduledSelected (100) (diff pages 25 Email from Each page)</t>
+  </si>
+  <si>
+    <t>Step 5: Reminders Scheduled Selected (100) (Total 999 reminders)</t>
+  </si>
+  <si>
+    <t>Cancel reminders(1000)</t>
+  </si>
+  <si>
+    <t>DMX Manual Readings - Cancel 1000 Reminders</t>
+  </si>
+  <si>
+    <t>Step 1: Cancel 1000 Reminders</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC46</t>
+  </si>
+  <si>
+    <t>Publish on Facebook</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC47</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC48</t>
+  </si>
+  <si>
+    <t>Publish on Twiiter</t>
+  </si>
+  <si>
+    <t>Publish on LinkedIn</t>
+  </si>
+  <si>
+    <t>Step 1: Facebook Post Preview</t>
+  </si>
+  <si>
+    <t>Step 2: Publish on Facebook</t>
+  </si>
+  <si>
+    <t>Step 1: Twiiter Post Preview</t>
+  </si>
+  <si>
+    <t>Step 2: Publish on Twitter</t>
+  </si>
+  <si>
+    <t>Step 1: LinkedIn Post Preview</t>
+  </si>
+  <si>
+    <t>Step 2: Publish on LinkedIn</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC49</t>
+  </si>
+  <si>
+    <t>Send SMS Invite wizard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 1: Enter Mobile Numbers </t>
+  </si>
+  <si>
+    <t>Step 2: Pre-Populate Survey</t>
+  </si>
+  <si>
+    <t>Step 3: Prepop mismatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 4: Customize SMS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 5: Preview SMS </t>
+  </si>
+  <si>
+    <t>Step 6: Send/Schedule Invitations</t>
+  </si>
+  <si>
+    <t>SMS invitation numbers.txt</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC45</t>
+  </si>
+  <si>
+    <t>I am proud to work at my school/~/Teaching gives me a feeling of accomplishment/~/Overall, I am satisfied with teaching/~/My current teaching duties are interesting/~/I am motivated to contribute more than what is expected of me at this school/~/I am not planning on leaving this school/~/I would feel comfortable referring a good friend to teach at this school/~/Overall, I enjoy working for this school’s principal</t>
+  </si>
+  <si>
+    <t>The school administrators make good decisions for the school overall/~/I enjoy the relationships I have with the school administrators/~/The classrooms where I teach are physically comfortable/~/My physical safety is protected at school/~/The school policies meet my needs as a teacher/~/The school supplies all the resources that I need to effectively teach my students/~/I fill a necessary role in the learning and growth of my students/~/I am a positive influence on my students</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>Step 5: Delete Same List</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC31</t>
-  </si>
-  <si>
-    <t>Offline invites for 999  records</t>
-  </si>
-  <si>
-    <t>Step 1: SAP Dashboard (Single URL)</t>
-  </si>
-  <si>
-    <t>Step 2: SAP Page</t>
-  </si>
-  <si>
-    <t>Step 3: Prepopulate survey</t>
-  </si>
-  <si>
-    <t>Step 4 : Template Selection Page</t>
-  </si>
-  <si>
-    <t>DMX Manual readings</t>
-  </si>
-  <si>
-    <t>1/~/2/~/3</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC32</t>
-  </si>
-  <si>
-    <t>DNT - Automation DMX Reading - Create New</t>
-  </si>
-  <si>
-    <t>Email Manager Tab wizard</t>
-  </si>
-  <si>
-    <t>Step 1: DM Page-Email Manager Tab</t>
-  </si>
-  <si>
-    <t>Step 2: Select an Email Template (Create New)</t>
-  </si>
-  <si>
-    <t>Step 3: Save the Template</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC33</t>
-  </si>
-  <si>
-    <t>Delete a Template Grid View</t>
-  </si>
-  <si>
-    <t>Step 1: Delete a Template Grid View</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC34</t>
-  </si>
-  <si>
-    <t>Delete a Template List View</t>
-  </si>
-  <si>
-    <t>Step 1: Delete a Template List View</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC35</t>
-  </si>
-  <si>
-    <t>Copy a Template Grid View</t>
-  </si>
-  <si>
-    <t>Step 1: Copy a Template Grid View</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC36</t>
-  </si>
-  <si>
-    <t>Copy a Template List View</t>
-  </si>
-  <si>
-    <t>Step 1: Copy a Template List View</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC37</t>
-  </si>
-  <si>
-    <t>Preview a Template Grid View</t>
-  </si>
-  <si>
-    <t>Step 1: Preview a Template Grid View</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC38</t>
-  </si>
-  <si>
-    <t>Preview a Template List View</t>
-  </si>
-  <si>
-    <t>Step 1: Preview a Template List View</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC39</t>
-  </si>
-  <si>
-    <t>Track survey Search 1 user</t>
-  </si>
-  <si>
-    <t>Step 1: Track survey page load</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step 2: Search record 1 </t>
-  </si>
-  <si>
-    <t>Step 3: Search record 2</t>
-  </si>
-  <si>
-    <t>channel</t>
-  </si>
-  <si>
-    <t>Single Use Link</t>
-  </si>
-  <si>
-    <t>searchRec1</t>
-  </si>
-  <si>
-    <t>searchRec2</t>
-  </si>
-  <si>
-    <t>kabirtest1@bluwberry.com291</t>
-  </si>
-  <si>
-    <t>kabirtest1@bluwberry.com292</t>
-  </si>
-  <si>
-    <t>textBox1</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC40</t>
-  </si>
-  <si>
-    <t>DELETE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Track survey Delete 100 records per page </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step 1: Track survey Page Deletion </t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC41</t>
-  </si>
-  <si>
-    <t>DNT- Automation DMX 999 list.xls</t>
-  </si>
-  <si>
-    <t>dateFormat</t>
-  </si>
-  <si>
-    <t>dd/mm/yyyy</t>
-  </si>
-  <si>
-    <t>Step 1: Schedule 999 records (By File)</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC42</t>
-  </si>
-  <si>
-    <t>Schedule 999 records (By List)</t>
-  </si>
-  <si>
-    <t>Step 1: Schedule 999 records (By List)</t>
-  </si>
-  <si>
-    <t>DNT- Automation DMX 999 list</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC43</t>
-  </si>
-  <si>
-    <t>Schedule 999 records (By File)</t>
-  </si>
-  <si>
-    <t>Schedule 999 records (Type Manually)</t>
-  </si>
-  <si>
-    <t>Step 1: Schedule 999 records (Type Manually)</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC44</t>
-  </si>
-  <si>
-    <t>Reminder Wizard (999 Invites in Surveys)</t>
-  </si>
-  <si>
-    <t>Step 1: Send/Schedule Reminder to all (Reminder Page)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step 2: Select Reminder Message </t>
-  </si>
-  <si>
-    <t>Step 4 : Reminders Send/Schedule ALL (999 reminders)</t>
-  </si>
-  <si>
-    <t>DMX Manual Readings (999 Invites)</t>
-  </si>
-  <si>
-    <t>Step 3: Schedule Reminders</t>
-  </si>
-  <si>
-    <t>Step 6: Reminders ScheduledSelected (100) (diff pages 25 Email from Each page)</t>
-  </si>
-  <si>
-    <t>Step 5: Reminders Scheduled Selected (100) (Total 999 reminders)</t>
-  </si>
-  <si>
-    <t>Cancel reminders(1000)</t>
-  </si>
-  <si>
-    <t>DMX Manual Readings - Cancel 1000 Reminders</t>
-  </si>
-  <si>
-    <t>Step 1: Cancel 1000 Reminders</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC46</t>
-  </si>
-  <si>
-    <t>Publish on Facebook</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC47</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC48</t>
-  </si>
-  <si>
-    <t>Publish on Twiiter</t>
-  </si>
-  <si>
-    <t>Publish on LinkedIn</t>
-  </si>
-  <si>
-    <t>Step 1: Facebook Post Preview</t>
-  </si>
-  <si>
-    <t>Step 2: Publish on Facebook</t>
-  </si>
-  <si>
-    <t>Step 1: Twiiter Post Preview</t>
-  </si>
-  <si>
-    <t>Step 2: Publish on Twitter</t>
-  </si>
-  <si>
-    <t>Step 1: LinkedIn Post Preview</t>
-  </si>
-  <si>
-    <t>Step 2: Publish on LinkedIn</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC49</t>
-  </si>
-  <si>
-    <t>Send SMS Invite wizard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step 1: Enter Mobile Numbers </t>
-  </si>
-  <si>
-    <t>Step 2: Pre-Populate Survey</t>
-  </si>
-  <si>
-    <t>Step 3: Prepop mismatch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step 4: Customize SMS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step 5: Preview SMS </t>
-  </si>
-  <si>
-    <t>Step 6: Send/Schedule Invitations</t>
-  </si>
-  <si>
-    <t>SMS invitation numbers.txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Template -21-Sep-2021 23:12:10 not present on page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Template -21-Sep-2021 23:52:50 not present on page.</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC45</t>
-  </si>
-  <si>
-    <t>I am proud to work at my school/~/Teaching gives me a feeling of accomplishment/~/Overall, I am satisfied with teaching/~/My current teaching duties are interesting/~/I am motivated to contribute more than what is expected of me at this school/~/I am not planning on leaving this school/~/I would feel comfortable referring a good friend to teach at this school/~/Overall, I enjoy working for this school’s principal</t>
-  </si>
-  <si>
-    <t>The school administrators make good decisions for the school overall/~/I enjoy the relationships I have with the school administrators/~/The classrooms where I teach are physically comfortable/~/My physical safety is protected at school/~/The school policies meet my needs as a teacher/~/The school supplies all the resources that I need to effectively teach my students/~/I fill a necessary role in the learning and growth of my students/~/I am a positive influence on my students</t>
+    <t>PlatformReadings_TC50</t>
+  </si>
+  <si>
+    <t>RMX</t>
+  </si>
+  <si>
+    <t>Publish</t>
+  </si>
+  <si>
+    <t>Response Rate Report</t>
+  </si>
+  <si>
+    <t>Step 1: Select Response Rate question</t>
+  </si>
+  <si>
+    <t>Step 2: Enter Maximum Count</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC51</t>
+  </si>
+  <si>
+    <t>Advance Frequency Report</t>
+  </si>
+  <si>
+    <t>Step 1: Select Survey Questions</t>
+  </si>
+  <si>
+    <t>Step 2: Re-order Questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 4:  Data Sources and Filters </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1165,39 +1188,8 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
   </fonts>
-  <fills count="19">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1245,51 +1237,6 @@
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1332,7 +1279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1349,18 +1296,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1651,8 +1591,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="42.85546875" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1707,9 +1647,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="60.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1745,15 +1685,15 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1786,7 +1726,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>48</v>
@@ -1824,25 +1764,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B22B77-F9A0-48CA-B95A-663324812831}">
-  <dimension ref="A1:BE50"/>
+  <dimension ref="A1:BE52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="11" max="56" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="56" width="14.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:57" x14ac:dyDescent="0.25">
@@ -1985,34 +1925,34 @@
         <v>215</v>
       </c>
       <c r="AU1" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AV1" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AW1" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AX1" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="AY1" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="AY1" s="3" t="s">
-        <v>245</v>
-      </c>
       <c r="AZ1" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="BA1" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="BA1" s="3" t="s">
-        <v>296</v>
-      </c>
       <c r="BB1" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="BC1" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="BD1" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="BE1" s="3" t="s">
         <v>21</v>
@@ -2023,7 +1963,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -2032,7 +1972,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>43</v>
@@ -2042,12 +1982,10 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>218</v>
-      </c>
+      <c r="J2" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
         <v>47</v>
       </c>
@@ -2125,7 +2063,7 @@
         <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>43</v>
@@ -2214,7 +2152,7 @@
         <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>43</v>
@@ -2303,7 +2241,7 @@
         <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>43</v>
@@ -2383,7 +2321,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -2392,7 +2330,7 @@
         <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>43</v>
@@ -2402,8 +2340,8 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="19" t="s">
-        <v>255</v>
+      <c r="J6" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5" t="s">
@@ -2497,7 +2435,7 @@
         <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>43</v>
@@ -2593,7 +2531,7 @@
         <v>75</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -2602,7 +2540,7 @@
         <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>43</v>
@@ -2612,8 +2550,8 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="20" t="s">
-        <v>255</v>
+      <c r="J8" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5" t="s">
@@ -2693,7 +2631,7 @@
         <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>43</v>
@@ -2786,7 +2724,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>43</v>
@@ -2879,7 +2817,7 @@
         <v>25</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>43</v>
@@ -2972,7 +2910,7 @@
         <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>43</v>
@@ -3065,7 +3003,7 @@
         <v>25</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>43</v>
@@ -3160,7 +3098,7 @@
         <v>25</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>43</v>
@@ -3255,7 +3193,7 @@
         <v>25</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>43</v>
@@ -3269,7 +3207,7 @@
         <v>27</v>
       </c>
       <c r="K15" s="5"/>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="12" t="s">
         <v>120</v>
       </c>
       <c r="M15" s="5">
@@ -3344,7 +3282,7 @@
         <v>25</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>43</v>
@@ -3425,7 +3363,7 @@
         <v>25</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>43</v>
@@ -3516,7 +3454,7 @@
         <v>25</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>43</v>
@@ -3609,7 +3547,7 @@
         <v>25</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>43</v>
@@ -3699,7 +3637,7 @@
         <v>141</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>13</v>
@@ -3708,7 +3646,7 @@
         <v>25</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>43</v>
@@ -3718,11 +3656,11 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="22" t="s">
-        <v>255</v>
+      <c r="J20" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="K20" s="5"/>
-      <c r="L20" s="5" t="s">
+      <c r="L20" s="12" t="s">
         <v>156</v>
       </c>
       <c r="M20" s="5">
@@ -3777,10 +3715,10 @@
       </c>
       <c r="AO20" s="1"/>
       <c r="AP20" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="AQ20" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="AR20" s="1"/>
       <c r="AS20" s="1"/>
@@ -3811,7 +3749,7 @@
         <v>25</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>43</v>
@@ -3910,7 +3848,7 @@
         <v>25</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>43</v>
@@ -4009,7 +3947,7 @@
         <v>25</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>43</v>
@@ -4100,7 +4038,7 @@
         <v>25</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>43</v>
@@ -4191,7 +4129,7 @@
         <v>25</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>43</v>
@@ -4293,15 +4231,15 @@
         <v>200</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>201</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="6"/>
-      <c r="J26" s="16" t="s">
-        <v>27</v>
+      <c r="J26" s="15" t="s">
+        <v>352</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5" t="s">
@@ -4362,7 +4300,7 @@
         <v>206</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>13</v>
@@ -4374,15 +4312,15 @@
         <v>200</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>207</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="6"/>
-      <c r="J27" s="17" t="s">
-        <v>255</v>
+      <c r="J27" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5" t="s">
@@ -4410,13 +4348,13 @@
         <v>217</v>
       </c>
       <c r="T27" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="V27" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="U27" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="V27" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="W27" s="7"/>
       <c r="X27" s="1"/>
@@ -4448,7 +4386,7 @@
       </c>
       <c r="AU27" s="9"/>
       <c r="AV27" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AW27" s="8"/>
       <c r="AX27" s="8"/>
@@ -4462,10 +4400,10 @@
     </row>
     <row r="28" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>13</v>
@@ -4477,10 +4415,10 @@
         <v>200</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="6"/>
@@ -4504,19 +4442,19 @@
         <v>212</v>
       </c>
       <c r="Q28" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="R28" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="R28" s="1" t="s">
+      <c r="S28" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="S28" s="1" t="s">
+      <c r="T28" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="T28" s="1" t="s">
+      <c r="U28" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="U28" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="V28" s="1"/>
       <c r="W28" s="7"/>
@@ -4546,10 +4484,10 @@
       </c>
       <c r="AT28" s="9"/>
       <c r="AU28" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AV28" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AW28" s="8"/>
       <c r="AX28" s="8"/>
@@ -4563,10 +4501,10 @@
     </row>
     <row r="29" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>13</v>
@@ -4578,15 +4516,15 @@
         <v>200</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="6"/>
-      <c r="J29" s="18" t="s">
-        <v>255</v>
+      <c r="J29" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="K29" s="5"/>
       <c r="L29" s="5" t="s">
@@ -4605,19 +4543,19 @@
         <v>212</v>
       </c>
       <c r="Q29" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="R29" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="R29" s="1" t="s">
+      <c r="S29" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="S29" s="1" t="s">
+      <c r="T29" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="T29" s="1" t="s">
+      <c r="U29" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="U29" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="V29" s="1"/>
       <c r="W29" s="7"/>
@@ -4647,10 +4585,10 @@
       </c>
       <c r="AT29" s="9"/>
       <c r="AU29" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AV29" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AW29" s="8"/>
       <c r="AX29" s="8"/>
@@ -4664,10 +4602,10 @@
     </row>
     <row r="30" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>13</v>
@@ -4679,10 +4617,10 @@
         <v>200</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="6"/>
@@ -4697,7 +4635,7 @@
         <v>890</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -4730,15 +4668,15 @@
       <c r="AQ30" s="1"/>
       <c r="AR30" s="2"/>
       <c r="AS30" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AT30" s="9"/>
       <c r="AU30" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AV30" s="8"/>
       <c r="AW30" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AX30" s="8"/>
       <c r="AY30" s="8"/>
@@ -4751,10 +4689,10 @@
     </row>
     <row r="31" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>13</v>
@@ -4766,10 +4704,10 @@
         <v>200</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="6"/>
@@ -4784,19 +4722,19 @@
         <v>890</v>
       </c>
       <c r="N31" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="P31" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="O31" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="P31" s="1" t="s">
+      <c r="Q31" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="Q31" s="1" t="s">
-        <v>251</v>
-      </c>
       <c r="R31" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
@@ -4827,15 +4765,15 @@
       <c r="AS31" s="9"/>
       <c r="AT31" s="9"/>
       <c r="AU31" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AV31" s="8"/>
       <c r="AW31" s="8"/>
       <c r="AX31" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AY31" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AZ31" s="8"/>
       <c r="BA31" s="8"/>
@@ -4846,10 +4784,10 @@
     </row>
     <row r="32" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>13</v>
@@ -4861,10 +4799,10 @@
         <v>200</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="6"/>
@@ -4879,16 +4817,16 @@
         <v>890</v>
       </c>
       <c r="N32" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="P32" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="Q32" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
@@ -4919,11 +4857,11 @@
       <c r="AR32" s="2"/>
       <c r="AS32" s="9"/>
       <c r="AT32" s="9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="AU32" s="9"/>
       <c r="AV32" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AW32" s="8"/>
       <c r="AX32" s="8"/>
@@ -4937,10 +4875,10 @@
     </row>
     <row r="33" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>13</v>
@@ -4952,10 +4890,10 @@
         <v>200</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="6"/>
@@ -4970,13 +4908,13 @@
         <v>890</v>
       </c>
       <c r="N33" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="P33" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>270</v>
       </c>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
@@ -5007,7 +4945,7 @@
       <c r="AQ33" s="1"/>
       <c r="AR33" s="2"/>
       <c r="AS33" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AT33" s="9"/>
       <c r="AU33" s="9"/>
@@ -5024,10 +4962,10 @@
     </row>
     <row r="34" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>13</v>
@@ -5039,19 +4977,17 @@
         <v>200</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="6"/>
-      <c r="J34" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>352</v>
-      </c>
+      <c r="J34" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K34" s="5"/>
       <c r="L34" s="5" t="s">
         <v>204</v>
       </c>
@@ -5059,7 +4995,7 @@
         <v>890</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
@@ -5092,7 +5028,7 @@
       <c r="AQ34" s="1"/>
       <c r="AR34" s="2"/>
       <c r="AS34" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AT34" s="9"/>
       <c r="AU34" s="9"/>
@@ -5109,10 +5045,10 @@
     </row>
     <row r="35" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>13</v>
@@ -5124,19 +5060,17 @@
         <v>200</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="6"/>
-      <c r="J35" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>351</v>
-      </c>
+      <c r="J35" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K35" s="5"/>
       <c r="L35" s="5" t="s">
         <v>204</v>
       </c>
@@ -5144,7 +5078,7 @@
         <v>890</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
@@ -5177,7 +5111,7 @@
       <c r="AQ35" s="1"/>
       <c r="AR35" s="2"/>
       <c r="AS35" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AT35" s="9"/>
       <c r="AU35" s="9"/>
@@ -5194,10 +5128,10 @@
     </row>
     <row r="36" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>13</v>
@@ -5209,10 +5143,10 @@
         <v>200</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="6"/>
@@ -5227,7 +5161,7 @@
         <v>890</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -5260,7 +5194,7 @@
       <c r="AQ36" s="1"/>
       <c r="AR36" s="2"/>
       <c r="AS36" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AT36" s="9"/>
       <c r="AU36" s="9"/>
@@ -5277,10 +5211,10 @@
     </row>
     <row r="37" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>13</v>
@@ -5292,10 +5226,10 @@
         <v>200</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="6"/>
@@ -5310,7 +5244,7 @@
         <v>890</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
@@ -5343,7 +5277,7 @@
       <c r="AQ37" s="1"/>
       <c r="AR37" s="2"/>
       <c r="AS37" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AT37" s="9"/>
       <c r="AU37" s="9"/>
@@ -5360,10 +5294,10 @@
     </row>
     <row r="38" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>13</v>
@@ -5375,10 +5309,10 @@
         <v>200</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="6"/>
@@ -5393,7 +5327,7 @@
         <v>890</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -5426,7 +5360,7 @@
       <c r="AQ38" s="1"/>
       <c r="AR38" s="2"/>
       <c r="AS38" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AT38" s="9"/>
       <c r="AU38" s="9"/>
@@ -5443,10 +5377,10 @@
     </row>
     <row r="39" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>13</v>
@@ -5458,10 +5392,10 @@
         <v>200</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="6"/>
@@ -5476,7 +5410,7 @@
         <v>890</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
@@ -5509,7 +5443,7 @@
       <c r="AQ39" s="1"/>
       <c r="AR39" s="2"/>
       <c r="AS39" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="AT39" s="9"/>
       <c r="AU39" s="9"/>
@@ -5526,10 +5460,10 @@
     </row>
     <row r="40" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>13</v>
@@ -5541,10 +5475,10 @@
         <v>200</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="6"/>
@@ -5559,13 +5493,13 @@
         <v>890</v>
       </c>
       <c r="N40" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="P40" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
@@ -5603,13 +5537,13 @@
       <c r="AX40" s="8"/>
       <c r="AY40" s="8"/>
       <c r="AZ40" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="BA40" s="10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="BB40" s="10" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="BC40" s="11"/>
       <c r="BD40" s="11"/>
@@ -5617,10 +5551,10 @@
     </row>
     <row r="41" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>13</v>
@@ -5632,10 +5566,10 @@
         <v>200</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="6"/>
@@ -5650,7 +5584,7 @@
         <v>890</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
@@ -5690,22 +5624,22 @@
       <c r="AX41" s="8"/>
       <c r="AY41" s="8"/>
       <c r="AZ41" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="BA41" s="10"/>
       <c r="BB41" s="10"/>
       <c r="BC41" s="11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="BD41" s="11"/>
       <c r="BE41" s="4"/>
     </row>
     <row r="42" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>13</v>
@@ -5717,10 +5651,10 @@
         <v>200</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="6"/>
@@ -5735,7 +5669,7 @@
         <v>890</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
@@ -5772,10 +5706,10 @@
       </c>
       <c r="AT42" s="9"/>
       <c r="AU42" s="9" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="AV42" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AW42" s="8"/>
       <c r="AX42" s="8"/>
@@ -5785,16 +5719,16 @@
       <c r="BB42" s="10"/>
       <c r="BC42" s="11"/>
       <c r="BD42" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="BE42" s="4"/>
     </row>
     <row r="43" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>13</v>
@@ -5806,10 +5740,10 @@
         <v>200</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="6"/>
@@ -5824,7 +5758,7 @@
         <v>890</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
@@ -5860,11 +5794,11 @@
         <v>209</v>
       </c>
       <c r="AT43" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="AU43" s="9"/>
       <c r="AV43" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AW43" s="8"/>
       <c r="AX43" s="8"/>
@@ -5874,16 +5808,16 @@
       <c r="BB43" s="10"/>
       <c r="BC43" s="11"/>
       <c r="BD43" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="BE43" s="4"/>
     </row>
     <row r="44" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>13</v>
@@ -5895,10 +5829,10 @@
         <v>200</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="6"/>
@@ -5913,7 +5847,7 @@
         <v>890</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
@@ -5950,10 +5884,10 @@
       </c>
       <c r="AT44" s="9"/>
       <c r="AU44" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AV44" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AW44" s="8"/>
       <c r="AX44" s="8"/>
@@ -5963,16 +5897,16 @@
       <c r="BB44" s="10"/>
       <c r="BC44" s="11"/>
       <c r="BD44" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="BE44" s="4"/>
     </row>
     <row r="45" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>13</v>
@@ -5984,10 +5918,10 @@
         <v>200</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="6"/>
@@ -5996,28 +5930,28 @@
       </c>
       <c r="K45" s="5"/>
       <c r="L45" s="12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="M45" s="5">
         <v>1288</v>
       </c>
       <c r="N45" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="Q45" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="O45" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="P45" s="1" t="s">
+      <c r="R45" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="Q45" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="R45" s="1" t="s">
-        <v>326</v>
-      </c>
       <c r="S45" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
@@ -6051,10 +5985,10 @@
       </c>
       <c r="AT45" s="9"/>
       <c r="AU45" s="9" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="AV45" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AW45" s="8"/>
       <c r="AX45" s="8"/>
@@ -6066,16 +6000,16 @@
         <v>4</v>
       </c>
       <c r="BD45" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="BE45" s="4"/>
     </row>
     <row r="46" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>13</v>
@@ -6087,25 +6021,25 @@
         <v>200</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="6"/>
-      <c r="J46" s="13" t="s">
-        <v>255</v>
+      <c r="J46" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="K46" s="5"/>
       <c r="L46" s="12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="M46" s="5">
         <v>1311</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
@@ -6142,10 +6076,10 @@
       </c>
       <c r="AT46" s="9"/>
       <c r="AU46" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AV46" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AW46" s="8"/>
       <c r="AX46" s="8"/>
@@ -6155,16 +6089,16 @@
       <c r="BB46" s="10"/>
       <c r="BC46" s="11"/>
       <c r="BD46" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="BE46" s="4"/>
     </row>
     <row r="47" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>13</v>
@@ -6176,10 +6110,10 @@
         <v>200</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="6"/>
@@ -6194,10 +6128,10 @@
         <v>890</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
@@ -6244,10 +6178,10 @@
     </row>
     <row r="48" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>13</v>
@@ -6259,10 +6193,10 @@
         <v>200</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="6"/>
@@ -6277,10 +6211,10 @@
         <v>890</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
@@ -6327,10 +6261,10 @@
     </row>
     <row r="49" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>13</v>
@@ -6342,10 +6276,10 @@
         <v>200</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="6"/>
@@ -6360,10 +6294,10 @@
         <v>890</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
@@ -6410,10 +6344,10 @@
     </row>
     <row r="50" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>13</v>
@@ -6425,10 +6359,10 @@
         <v>200</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>200</v>
+        <v>355</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="6"/>
@@ -6443,22 +6377,22 @@
         <v>890</v>
       </c>
       <c r="N50" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="P50" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="O50" s="1" t="s">
+      <c r="Q50" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="P50" s="1" t="s">
+      <c r="R50" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="Q50" s="1" t="s">
+      <c r="S50" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="R50" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="S50" s="1" t="s">
-        <v>349</v>
       </c>
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
@@ -6488,7 +6422,7 @@
       <c r="AS50" s="9"/>
       <c r="AT50" s="9"/>
       <c r="AU50" s="9" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AV50" s="8"/>
       <c r="AW50" s="8"/>
@@ -6500,6 +6434,184 @@
       <c r="BC50" s="11"/>
       <c r="BD50" s="11"/>
       <c r="BE50" s="4"/>
+    </row>
+    <row r="51" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="H51" s="1"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M51" s="5">
+        <v>527</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q51" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="7"/>
+      <c r="X51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y51" s="1"/>
+      <c r="Z51" s="1"/>
+      <c r="AA51" s="1"/>
+      <c r="AB51" s="1"/>
+      <c r="AC51" s="1"/>
+      <c r="AD51" s="1"/>
+      <c r="AE51" s="1"/>
+      <c r="AF51" s="1"/>
+      <c r="AG51" s="1"/>
+      <c r="AH51" s="7"/>
+      <c r="AI51" s="8"/>
+      <c r="AJ51" s="8"/>
+      <c r="AK51" s="1"/>
+      <c r="AL51" s="1"/>
+      <c r="AM51" s="1"/>
+      <c r="AN51" s="1"/>
+      <c r="AO51" s="1"/>
+      <c r="AP51" s="1"/>
+      <c r="AQ51" s="1"/>
+      <c r="AR51" s="2"/>
+      <c r="AS51" s="9"/>
+      <c r="AT51" s="9"/>
+      <c r="AU51" s="9"/>
+      <c r="AV51" s="8"/>
+      <c r="AW51" s="8"/>
+      <c r="AX51" s="8"/>
+      <c r="AY51" s="8"/>
+      <c r="AZ51" s="8"/>
+      <c r="BA51" s="10"/>
+      <c r="BB51" s="10"/>
+      <c r="BC51" s="11"/>
+      <c r="BD51" s="11"/>
+      <c r="BE51" s="4"/>
+    </row>
+    <row r="52" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="H52" s="1"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M52" s="5">
+        <v>527</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q52" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="R52" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="7"/>
+      <c r="X52" s="1"/>
+      <c r="Y52" s="1"/>
+      <c r="Z52" s="1"/>
+      <c r="AA52" s="1"/>
+      <c r="AB52" s="1"/>
+      <c r="AC52" s="1"/>
+      <c r="AD52" s="1"/>
+      <c r="AE52" s="1"/>
+      <c r="AF52" s="1"/>
+      <c r="AG52" s="1"/>
+      <c r="AH52" s="7"/>
+      <c r="AI52" s="8"/>
+      <c r="AJ52" s="8"/>
+      <c r="AK52" s="1"/>
+      <c r="AL52" s="1"/>
+      <c r="AM52" s="1"/>
+      <c r="AN52" s="1"/>
+      <c r="AO52" s="1"/>
+      <c r="AP52" s="1"/>
+      <c r="AQ52" s="1"/>
+      <c r="AR52" s="2"/>
+      <c r="AS52" s="9"/>
+      <c r="AT52" s="9"/>
+      <c r="AU52" s="9"/>
+      <c r="AV52" s="8"/>
+      <c r="AW52" s="8"/>
+      <c r="AX52" s="8"/>
+      <c r="AY52" s="8"/>
+      <c r="AZ52" s="8"/>
+      <c r="BA52" s="10"/>
+      <c r="BB52" s="10"/>
+      <c r="BC52" s="11"/>
+      <c r="BD52" s="11"/>
+      <c r="BE52" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Data readings added and new dashboard issues been resolved in performance suite.
</commit_message>
<xml_diff>
--- a/Engage/Engage-Performance/src/main/resources/excelfiles/Engage_PlatformReadings.xlsx
+++ b/Engage/Engage-Performance/src/main/resources/excelfiles/Engage_PlatformReadings.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BA1057-F6EF-44F8-B0A0-BCE9A4670454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E4898E-0594-40AB-A865-1E9488971819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="412">
   <si>
     <t>Environment</t>
   </si>
@@ -1115,13 +1115,157 @@
   </si>
   <si>
     <t xml:space="preserve">Step 4:  Data Sources and Filters </t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>gjoy_test</t>
+  </si>
+  <si>
+    <t>Eighth8#</t>
+  </si>
+  <si>
+    <t>toggleData</t>
+  </si>
+  <si>
+    <t>fromDate</t>
+  </si>
+  <si>
+    <t>toDate</t>
+  </si>
+  <si>
+    <t>respPeriodCond</t>
+  </si>
+  <si>
+    <t>IP,emailAddr,browserType,OS,screenRes,startEndTime</t>
+  </si>
+  <si>
+    <t>01-Jan-2018</t>
+  </si>
+  <si>
+    <t>07-Dec-2021</t>
+  </si>
+  <si>
+    <t>Between</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC52</t>
+  </si>
+  <si>
+    <t>Home Page to Data Module</t>
+  </si>
+  <si>
+    <t>All Q Survey Fruits EXE after 17.0 live</t>
+  </si>
+  <si>
+    <t>Step 1: Navigate to Data module from Home Page using 'All survey Dashboard'.</t>
+  </si>
+  <si>
+    <t>Step 2: Navigate to Data module from Home Page using Data module icon from Recent Surveys.</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC53</t>
+  </si>
+  <si>
+    <t>Export Excel</t>
+  </si>
+  <si>
+    <t>Step 1: Select Excel format</t>
+  </si>
+  <si>
+    <t>Step 2: Select Survey Questions and Click Continue.</t>
+  </si>
+  <si>
+    <t>Step 3: Toggle 'ON' all Respondent Attributes and Response Attributes  and Click Continue.</t>
+  </si>
+  <si>
+    <t>Step 4: Apply 1 condition and any Date filter and Click Continue.</t>
+  </si>
+  <si>
+    <t>Step 5:  Toggle 'ON' Assign code and Click Continue.</t>
+  </si>
+  <si>
+    <t>Q1. What's your Name?</t>
+  </si>
+  <si>
+    <t>contains</t>
+  </si>
+  <si>
+    <t>Godwin</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC54</t>
+  </si>
+  <si>
+    <t>Export CSV</t>
+  </si>
+  <si>
+    <t>Step 1: Select CSV format</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC55</t>
+  </si>
+  <si>
+    <t>Export XML</t>
+  </si>
+  <si>
+    <t>Step 1: Select XML format</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC56</t>
+  </si>
+  <si>
+    <t>Export Access</t>
+  </si>
+  <si>
+    <t>Step 1: Select Access format</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC57</t>
+  </si>
+  <si>
+    <t>Export Word</t>
+  </si>
+  <si>
+    <t>Step 1: Select Word format</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC58</t>
+  </si>
+  <si>
+    <t>Export HTML</t>
+  </si>
+  <si>
+    <t>Step 1: Select HTML format</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC59</t>
+  </si>
+  <si>
+    <t>Export SPSS</t>
+  </si>
+  <si>
+    <t>Step 1: Select SPSS format</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC60</t>
+  </si>
+  <si>
+    <t>Export SoGo1</t>
+  </si>
+  <si>
+    <t>Step 1: Export SoGo</t>
+  </si>
+  <si>
+    <t>Step 6: Click any range and click Export. (Note the time until download is completed)*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1183,13 +1327,8 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1209,27 +1348,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="17"/>
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
       </patternFill>
     </fill>
     <fill>
@@ -1279,7 +1403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1295,12 +1419,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="6" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1682,10 +1805,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,22 +1875,37 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{59B4C049-04B3-4447-9A04-941BCA3EDEAB}"/>
+    <hyperlink ref="C5" r:id="rId2" display="Welcome@1234" xr:uid="{0F84803B-12AB-4CAA-B366-DC666824EAA6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B22B77-F9A0-48CA-B95A-663324812831}">
-  <dimension ref="A1:BE52"/>
+  <dimension ref="A1:BI61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView tabSelected="1" topLeftCell="M49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R64" sqref="R64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1782,10 +1920,10 @@
     <col min="8" max="8" width="16" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="56" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="60" width="14.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -1955,15 +2093,27 @@
         <v>305</v>
       </c>
       <c r="BE1" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="BF1" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="BG1" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="BH1" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="BI1" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -1982,8 +2132,8 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="13" t="s">
-        <v>352</v>
+      <c r="J2" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
@@ -2047,9 +2197,13 @@
       <c r="BB2" s="1"/>
       <c r="BC2" s="1"/>
       <c r="BD2" s="1"/>
-      <c r="BE2" s="4"/>
+      <c r="BE2" s="1"/>
+      <c r="BF2" s="1"/>
+      <c r="BG2" s="1"/>
+      <c r="BH2" s="1"/>
+      <c r="BI2" s="4"/>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -2073,7 +2227,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K3" s="5"/>
@@ -2136,9 +2290,13 @@
       <c r="BB3" s="1"/>
       <c r="BC3" s="1"/>
       <c r="BD3" s="1"/>
-      <c r="BE3" s="4"/>
+      <c r="BE3" s="1"/>
+      <c r="BF3" s="1"/>
+      <c r="BG3" s="1"/>
+      <c r="BH3" s="1"/>
+      <c r="BI3" s="4"/>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -2162,7 +2320,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K4" s="5"/>
@@ -2225,9 +2383,13 @@
       <c r="BB4" s="1"/>
       <c r="BC4" s="1"/>
       <c r="BD4" s="1"/>
-      <c r="BE4" s="4"/>
+      <c r="BE4" s="1"/>
+      <c r="BF4" s="1"/>
+      <c r="BG4" s="1"/>
+      <c r="BH4" s="1"/>
+      <c r="BI4" s="4"/>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -2251,7 +2413,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="5"/>
@@ -2314,9 +2476,13 @@
       <c r="BB5" s="1"/>
       <c r="BC5" s="1"/>
       <c r="BD5" s="1"/>
-      <c r="BE5" s="4"/>
+      <c r="BE5" s="1"/>
+      <c r="BF5" s="1"/>
+      <c r="BG5" s="1"/>
+      <c r="BH5" s="1"/>
+      <c r="BI5" s="4"/>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -2340,7 +2506,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K6" s="5"/>
@@ -2419,9 +2585,13 @@
       <c r="BB6" s="1"/>
       <c r="BC6" s="1"/>
       <c r="BD6" s="1"/>
-      <c r="BE6" s="4"/>
+      <c r="BE6" s="1"/>
+      <c r="BF6" s="1"/>
+      <c r="BG6" s="1"/>
+      <c r="BH6" s="1"/>
+      <c r="BI6" s="4"/>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>72</v>
       </c>
@@ -2445,7 +2615,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="6"/>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K7" s="5"/>
@@ -2524,9 +2694,13 @@
       <c r="BB7" s="1"/>
       <c r="BC7" s="1"/>
       <c r="BD7" s="1"/>
-      <c r="BE7" s="4"/>
+      <c r="BE7" s="1"/>
+      <c r="BF7" s="1"/>
+      <c r="BG7" s="1"/>
+      <c r="BH7" s="1"/>
+      <c r="BI7" s="4"/>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>75</v>
       </c>
@@ -2550,7 +2724,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K8" s="5"/>
@@ -2615,9 +2789,13 @@
       <c r="BB8" s="1"/>
       <c r="BC8" s="1"/>
       <c r="BD8" s="1"/>
-      <c r="BE8" s="4"/>
+      <c r="BE8" s="1"/>
+      <c r="BF8" s="1"/>
+      <c r="BG8" s="1"/>
+      <c r="BH8" s="1"/>
+      <c r="BI8" s="4"/>
     </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>84</v>
       </c>
@@ -2641,7 +2819,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K9" s="5"/>
@@ -2708,9 +2886,13 @@
       <c r="BB9" s="1"/>
       <c r="BC9" s="1"/>
       <c r="BD9" s="1"/>
-      <c r="BE9" s="4"/>
+      <c r="BE9" s="1"/>
+      <c r="BF9" s="1"/>
+      <c r="BG9" s="1"/>
+      <c r="BH9" s="1"/>
+      <c r="BI9" s="4"/>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>89</v>
       </c>
@@ -2734,7 +2916,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K10" s="5"/>
@@ -2801,9 +2983,13 @@
       <c r="BB10" s="1"/>
       <c r="BC10" s="1"/>
       <c r="BD10" s="1"/>
-      <c r="BE10" s="4"/>
+      <c r="BE10" s="1"/>
+      <c r="BF10" s="1"/>
+      <c r="BG10" s="1"/>
+      <c r="BH10" s="1"/>
+      <c r="BI10" s="4"/>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>92</v>
       </c>
@@ -2827,7 +3013,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K11" s="5"/>
@@ -2894,9 +3080,13 @@
       <c r="BB11" s="1"/>
       <c r="BC11" s="1"/>
       <c r="BD11" s="1"/>
-      <c r="BE11" s="4"/>
+      <c r="BE11" s="1"/>
+      <c r="BF11" s="1"/>
+      <c r="BG11" s="1"/>
+      <c r="BH11" s="1"/>
+      <c r="BI11" s="4"/>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>95</v>
       </c>
@@ -2920,7 +3110,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K12" s="5"/>
@@ -2987,9 +3177,13 @@
       <c r="BB12" s="1"/>
       <c r="BC12" s="1"/>
       <c r="BD12" s="1"/>
-      <c r="BE12" s="4"/>
+      <c r="BE12" s="1"/>
+      <c r="BF12" s="1"/>
+      <c r="BG12" s="1"/>
+      <c r="BH12" s="1"/>
+      <c r="BI12" s="4"/>
     </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>104</v>
       </c>
@@ -3013,7 +3207,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K13" s="5"/>
@@ -3082,9 +3276,13 @@
       <c r="BB13" s="7"/>
       <c r="BC13" s="7"/>
       <c r="BD13" s="7"/>
-      <c r="BE13" s="4"/>
+      <c r="BE13" s="7"/>
+      <c r="BF13" s="7"/>
+      <c r="BG13" s="7"/>
+      <c r="BH13" s="7"/>
+      <c r="BI13" s="4"/>
     </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>107</v>
       </c>
@@ -3108,7 +3306,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K14" s="5"/>
@@ -3177,9 +3375,13 @@
       <c r="BB14" s="8"/>
       <c r="BC14" s="8"/>
       <c r="BD14" s="8"/>
-      <c r="BE14" s="4"/>
+      <c r="BE14" s="1"/>
+      <c r="BF14" s="1"/>
+      <c r="BG14" s="1"/>
+      <c r="BH14" s="1"/>
+      <c r="BI14" s="4"/>
     </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>118</v>
       </c>
@@ -3203,7 +3405,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="14" t="s">
+      <c r="J15" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K15" s="5"/>
@@ -3266,9 +3468,13 @@
       <c r="BB15" s="8"/>
       <c r="BC15" s="8"/>
       <c r="BD15" s="8"/>
-      <c r="BE15" s="4"/>
+      <c r="BE15" s="1"/>
+      <c r="BF15" s="1"/>
+      <c r="BG15" s="1"/>
+      <c r="BH15" s="1"/>
+      <c r="BI15" s="4"/>
     </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>121</v>
       </c>
@@ -3292,7 +3498,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="14" t="s">
+      <c r="J16" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K16" s="5"/>
@@ -3347,9 +3553,13 @@
       <c r="BB16" s="8"/>
       <c r="BC16" s="8"/>
       <c r="BD16" s="8"/>
-      <c r="BE16" s="4"/>
+      <c r="BE16" s="1"/>
+      <c r="BF16" s="1"/>
+      <c r="BG16" s="1"/>
+      <c r="BH16" s="1"/>
+      <c r="BI16" s="4"/>
     </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>123</v>
       </c>
@@ -3373,7 +3583,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K17" s="5"/>
@@ -3438,9 +3648,13 @@
       <c r="BB17" s="8"/>
       <c r="BC17" s="8"/>
       <c r="BD17" s="8"/>
-      <c r="BE17" s="4"/>
+      <c r="BE17" s="1"/>
+      <c r="BF17" s="1"/>
+      <c r="BG17" s="1"/>
+      <c r="BH17" s="1"/>
+      <c r="BI17" s="4"/>
     </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>128</v>
       </c>
@@ -3464,7 +3678,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="14" t="s">
+      <c r="J18" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K18" s="5"/>
@@ -3531,9 +3745,13 @@
       <c r="BB18" s="8"/>
       <c r="BC18" s="8"/>
       <c r="BD18" s="8"/>
-      <c r="BE18" s="4"/>
+      <c r="BE18" s="1"/>
+      <c r="BF18" s="1"/>
+      <c r="BG18" s="1"/>
+      <c r="BH18" s="1"/>
+      <c r="BI18" s="4"/>
     </row>
-    <row r="19" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>131</v>
       </c>
@@ -3557,7 +3775,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="14" t="s">
+      <c r="J19" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K19" s="5"/>
@@ -3630,9 +3848,13 @@
       <c r="BB19" s="1"/>
       <c r="BC19" s="1"/>
       <c r="BD19" s="1"/>
-      <c r="BE19" s="4"/>
+      <c r="BE19" s="1"/>
+      <c r="BF19" s="1"/>
+      <c r="BG19" s="1"/>
+      <c r="BH19" s="1"/>
+      <c r="BI19" s="4"/>
     </row>
-    <row r="20" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>141</v>
       </c>
@@ -3656,7 +3878,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="14" t="s">
+      <c r="J20" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K20" s="5"/>
@@ -3733,9 +3955,13 @@
       <c r="BB20" s="1"/>
       <c r="BC20" s="1"/>
       <c r="BD20" s="1"/>
-      <c r="BE20" s="4"/>
+      <c r="BE20" s="1"/>
+      <c r="BF20" s="1"/>
+      <c r="BG20" s="1"/>
+      <c r="BH20" s="1"/>
+      <c r="BI20" s="4"/>
     </row>
-    <row r="21" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>159</v>
       </c>
@@ -3759,7 +3985,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="6"/>
-      <c r="J21" s="14" t="s">
+      <c r="J21" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K21" s="5"/>
@@ -3832,9 +4058,13 @@
       <c r="BB21" s="1"/>
       <c r="BC21" s="1"/>
       <c r="BD21" s="1"/>
-      <c r="BE21" s="4"/>
+      <c r="BE21" s="1"/>
+      <c r="BF21" s="1"/>
+      <c r="BG21" s="1"/>
+      <c r="BH21" s="1"/>
+      <c r="BI21" s="4"/>
     </row>
-    <row r="22" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>174</v>
       </c>
@@ -3858,7 +4088,7 @@
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="6"/>
-      <c r="J22" s="14" t="s">
+      <c r="J22" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K22" s="5"/>
@@ -3931,9 +4161,13 @@
       <c r="BB22" s="1"/>
       <c r="BC22" s="1"/>
       <c r="BD22" s="1"/>
-      <c r="BE22" s="4"/>
+      <c r="BE22" s="1"/>
+      <c r="BF22" s="1"/>
+      <c r="BG22" s="1"/>
+      <c r="BH22" s="1"/>
+      <c r="BI22" s="4"/>
     </row>
-    <row r="23" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>175</v>
       </c>
@@ -3957,7 +4191,7 @@
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="6"/>
-      <c r="J23" s="14" t="s">
+      <c r="J23" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K23" s="5"/>
@@ -4022,9 +4256,13 @@
       <c r="BB23" s="1"/>
       <c r="BC23" s="1"/>
       <c r="BD23" s="1"/>
-      <c r="BE23" s="4"/>
+      <c r="BE23" s="1"/>
+      <c r="BF23" s="1"/>
+      <c r="BG23" s="1"/>
+      <c r="BH23" s="1"/>
+      <c r="BI23" s="4"/>
     </row>
-    <row r="24" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>181</v>
       </c>
@@ -4048,7 +4286,7 @@
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="6"/>
-      <c r="J24" s="14" t="s">
+      <c r="J24" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K24" s="5"/>
@@ -4113,9 +4351,13 @@
       <c r="BB24" s="1"/>
       <c r="BC24" s="1"/>
       <c r="BD24" s="1"/>
-      <c r="BE24" s="4"/>
+      <c r="BE24" s="1"/>
+      <c r="BF24" s="1"/>
+      <c r="BG24" s="1"/>
+      <c r="BH24" s="1"/>
+      <c r="BI24" s="4"/>
     </row>
-    <row r="25" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>188</v>
       </c>
@@ -4139,7 +4381,7 @@
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="6"/>
-      <c r="J25" s="14" t="s">
+      <c r="J25" s="15" t="s">
         <v>27</v>
       </c>
       <c r="K25" s="5"/>
@@ -4212,14 +4454,18 @@
       <c r="BB25" s="2"/>
       <c r="BC25" s="2"/>
       <c r="BD25" s="2"/>
-      <c r="BE25" s="4"/>
+      <c r="BE25" s="2"/>
+      <c r="BF25" s="2"/>
+      <c r="BG25" s="2"/>
+      <c r="BH25" s="2"/>
+      <c r="BI25" s="4"/>
     </row>
-    <row r="26" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>199</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>13</v>
@@ -4238,8 +4484,8 @@
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="6"/>
-      <c r="J26" s="15" t="s">
-        <v>352</v>
+      <c r="J26" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5" t="s">
@@ -4293,9 +4539,13 @@
       <c r="BB26" s="2"/>
       <c r="BC26" s="2"/>
       <c r="BD26" s="2"/>
-      <c r="BE26" s="4"/>
+      <c r="BE26" s="2"/>
+      <c r="BF26" s="2"/>
+      <c r="BG26" s="2"/>
+      <c r="BH26" s="2"/>
+      <c r="BI26" s="4"/>
     </row>
-    <row r="27" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>206</v>
       </c>
@@ -4396,9 +4646,13 @@
       <c r="BB27" s="8"/>
       <c r="BC27" s="8"/>
       <c r="BD27" s="8"/>
-      <c r="BE27" s="4"/>
+      <c r="BE27" s="1"/>
+      <c r="BF27" s="1"/>
+      <c r="BG27" s="1"/>
+      <c r="BH27" s="1"/>
+      <c r="BI27" s="4"/>
     </row>
-    <row r="28" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>223</v>
       </c>
@@ -4497,9 +4751,13 @@
       <c r="BB28" s="8"/>
       <c r="BC28" s="8"/>
       <c r="BD28" s="8"/>
-      <c r="BE28" s="4"/>
+      <c r="BE28" s="1"/>
+      <c r="BF28" s="1"/>
+      <c r="BG28" s="1"/>
+      <c r="BH28" s="1"/>
+      <c r="BI28" s="4"/>
     </row>
-    <row r="29" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>233</v>
       </c>
@@ -4598,9 +4856,13 @@
       <c r="BB29" s="8"/>
       <c r="BC29" s="8"/>
       <c r="BD29" s="8"/>
-      <c r="BE29" s="4"/>
+      <c r="BE29" s="1"/>
+      <c r="BF29" s="1"/>
+      <c r="BG29" s="1"/>
+      <c r="BH29" s="1"/>
+      <c r="BI29" s="4"/>
     </row>
-    <row r="30" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>236</v>
       </c>
@@ -4685,9 +4947,13 @@
       <c r="BB30" s="8"/>
       <c r="BC30" s="8"/>
       <c r="BD30" s="8"/>
-      <c r="BE30" s="4"/>
+      <c r="BE30" s="1"/>
+      <c r="BF30" s="1"/>
+      <c r="BG30" s="1"/>
+      <c r="BH30" s="1"/>
+      <c r="BI30" s="4"/>
     </row>
-    <row r="31" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>252</v>
       </c>
@@ -4780,9 +5046,13 @@
       <c r="BB31" s="8"/>
       <c r="BC31" s="8"/>
       <c r="BD31" s="8"/>
-      <c r="BE31" s="4"/>
+      <c r="BE31" s="1"/>
+      <c r="BF31" s="1"/>
+      <c r="BG31" s="1"/>
+      <c r="BH31" s="1"/>
+      <c r="BI31" s="4"/>
     </row>
-    <row r="32" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>255</v>
       </c>
@@ -4871,9 +5141,13 @@
       <c r="BB32" s="8"/>
       <c r="BC32" s="8"/>
       <c r="BD32" s="8"/>
-      <c r="BE32" s="4"/>
+      <c r="BE32" s="1"/>
+      <c r="BF32" s="1"/>
+      <c r="BG32" s="1"/>
+      <c r="BH32" s="1"/>
+      <c r="BI32" s="4"/>
     </row>
-    <row r="33" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>263</v>
       </c>
@@ -4958,9 +5232,13 @@
       <c r="BB33" s="8"/>
       <c r="BC33" s="8"/>
       <c r="BD33" s="8"/>
-      <c r="BE33" s="4"/>
+      <c r="BE33" s="1"/>
+      <c r="BF33" s="1"/>
+      <c r="BG33" s="1"/>
+      <c r="BH33" s="1"/>
+      <c r="BI33" s="4"/>
     </row>
-    <row r="34" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>269</v>
       </c>
@@ -5041,9 +5319,13 @@
       <c r="BB34" s="8"/>
       <c r="BC34" s="8"/>
       <c r="BD34" s="8"/>
-      <c r="BE34" s="4"/>
+      <c r="BE34" s="1"/>
+      <c r="BF34" s="1"/>
+      <c r="BG34" s="1"/>
+      <c r="BH34" s="1"/>
+      <c r="BI34" s="4"/>
     </row>
-    <row r="35" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>272</v>
       </c>
@@ -5124,9 +5406,13 @@
       <c r="BB35" s="8"/>
       <c r="BC35" s="8"/>
       <c r="BD35" s="8"/>
-      <c r="BE35" s="4"/>
+      <c r="BE35" s="1"/>
+      <c r="BF35" s="1"/>
+      <c r="BG35" s="1"/>
+      <c r="BH35" s="1"/>
+      <c r="BI35" s="4"/>
     </row>
-    <row r="36" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>275</v>
       </c>
@@ -5207,9 +5493,13 @@
       <c r="BB36" s="8"/>
       <c r="BC36" s="8"/>
       <c r="BD36" s="8"/>
-      <c r="BE36" s="4"/>
+      <c r="BE36" s="1"/>
+      <c r="BF36" s="1"/>
+      <c r="BG36" s="1"/>
+      <c r="BH36" s="1"/>
+      <c r="BI36" s="4"/>
     </row>
-    <row r="37" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>278</v>
       </c>
@@ -5290,9 +5580,13 @@
       <c r="BB37" s="8"/>
       <c r="BC37" s="8"/>
       <c r="BD37" s="8"/>
-      <c r="BE37" s="4"/>
+      <c r="BE37" s="1"/>
+      <c r="BF37" s="1"/>
+      <c r="BG37" s="1"/>
+      <c r="BH37" s="1"/>
+      <c r="BI37" s="4"/>
     </row>
-    <row r="38" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>281</v>
       </c>
@@ -5373,9 +5667,13 @@
       <c r="BB38" s="8"/>
       <c r="BC38" s="8"/>
       <c r="BD38" s="8"/>
-      <c r="BE38" s="4"/>
+      <c r="BE38" s="1"/>
+      <c r="BF38" s="1"/>
+      <c r="BG38" s="1"/>
+      <c r="BH38" s="1"/>
+      <c r="BI38" s="4"/>
     </row>
-    <row r="39" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>284</v>
       </c>
@@ -5456,9 +5754,13 @@
       <c r="BB39" s="8"/>
       <c r="BC39" s="8"/>
       <c r="BD39" s="8"/>
-      <c r="BE39" s="4"/>
+      <c r="BE39" s="1"/>
+      <c r="BF39" s="1"/>
+      <c r="BG39" s="1"/>
+      <c r="BH39" s="1"/>
+      <c r="BI39" s="4"/>
     </row>
-    <row r="40" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>287</v>
       </c>
@@ -5547,9 +5849,13 @@
       </c>
       <c r="BC40" s="11"/>
       <c r="BD40" s="11"/>
-      <c r="BE40" s="4"/>
+      <c r="BE40" s="11"/>
+      <c r="BF40" s="11"/>
+      <c r="BG40" s="11"/>
+      <c r="BH40" s="11"/>
+      <c r="BI40" s="4"/>
     </row>
-    <row r="41" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>299</v>
       </c>
@@ -5632,9 +5938,13 @@
         <v>300</v>
       </c>
       <c r="BD41" s="11"/>
-      <c r="BE41" s="4"/>
+      <c r="BE41" s="11"/>
+      <c r="BF41" s="11"/>
+      <c r="BG41" s="11"/>
+      <c r="BH41" s="11"/>
+      <c r="BI41" s="4"/>
     </row>
-    <row r="42" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>303</v>
       </c>
@@ -5721,9 +6031,13 @@
       <c r="BD42" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="BE42" s="4"/>
+      <c r="BE42" s="11"/>
+      <c r="BF42" s="11"/>
+      <c r="BG42" s="11"/>
+      <c r="BH42" s="11"/>
+      <c r="BI42" s="4"/>
     </row>
-    <row r="43" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>308</v>
       </c>
@@ -5810,9 +6124,13 @@
       <c r="BD43" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="BE43" s="4"/>
+      <c r="BE43" s="11"/>
+      <c r="BF43" s="11"/>
+      <c r="BG43" s="11"/>
+      <c r="BH43" s="11"/>
+      <c r="BI43" s="4"/>
     </row>
-    <row r="44" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>312</v>
       </c>
@@ -5899,9 +6217,13 @@
       <c r="BD44" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="BE44" s="4"/>
+      <c r="BE44" s="11"/>
+      <c r="BF44" s="11"/>
+      <c r="BG44" s="11"/>
+      <c r="BH44" s="11"/>
+      <c r="BI44" s="4"/>
     </row>
-    <row r="45" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>316</v>
       </c>
@@ -6002,9 +6324,13 @@
       <c r="BD45" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="BE45" s="4"/>
+      <c r="BE45" s="11"/>
+      <c r="BF45" s="11"/>
+      <c r="BG45" s="11"/>
+      <c r="BH45" s="11"/>
+      <c r="BI45" s="4"/>
     </row>
-    <row r="46" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>349</v>
       </c>
@@ -6091,9 +6417,13 @@
       <c r="BD46" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="BE46" s="4"/>
+      <c r="BE46" s="11"/>
+      <c r="BF46" s="11"/>
+      <c r="BG46" s="11"/>
+      <c r="BH46" s="11"/>
+      <c r="BI46" s="4"/>
     </row>
-    <row r="47" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>328</v>
       </c>
@@ -6174,9 +6504,13 @@
       <c r="BB47" s="10"/>
       <c r="BC47" s="11"/>
       <c r="BD47" s="11"/>
-      <c r="BE47" s="4"/>
+      <c r="BE47" s="11"/>
+      <c r="BF47" s="11"/>
+      <c r="BG47" s="11"/>
+      <c r="BH47" s="11"/>
+      <c r="BI47" s="4"/>
     </row>
-    <row r="48" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>330</v>
       </c>
@@ -6257,9 +6591,13 @@
       <c r="BB48" s="10"/>
       <c r="BC48" s="11"/>
       <c r="BD48" s="11"/>
-      <c r="BE48" s="4"/>
+      <c r="BE48" s="11"/>
+      <c r="BF48" s="11"/>
+      <c r="BG48" s="11"/>
+      <c r="BH48" s="11"/>
+      <c r="BI48" s="4"/>
     </row>
-    <row r="49" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>331</v>
       </c>
@@ -6340,9 +6678,13 @@
       <c r="BB49" s="10"/>
       <c r="BC49" s="11"/>
       <c r="BD49" s="11"/>
-      <c r="BE49" s="4"/>
+      <c r="BE49" s="11"/>
+      <c r="BF49" s="11"/>
+      <c r="BG49" s="11"/>
+      <c r="BH49" s="11"/>
+      <c r="BI49" s="4"/>
     </row>
-    <row r="50" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>340</v>
       </c>
@@ -6433,14 +6775,18 @@
       <c r="BB50" s="10"/>
       <c r="BC50" s="11"/>
       <c r="BD50" s="11"/>
-      <c r="BE50" s="4"/>
+      <c r="BE50" s="11"/>
+      <c r="BF50" s="11"/>
+      <c r="BG50" s="11"/>
+      <c r="BH50" s="11"/>
+      <c r="BI50" s="4"/>
     </row>
-    <row r="51" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>353</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>13</v>
@@ -6459,8 +6805,8 @@
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="6"/>
-      <c r="J51" s="17" t="s">
-        <v>352</v>
+      <c r="J51" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="K51" s="5"/>
       <c r="L51" s="5" t="s">
@@ -6522,14 +6868,18 @@
       <c r="BB51" s="10"/>
       <c r="BC51" s="11"/>
       <c r="BD51" s="11"/>
-      <c r="BE51" s="4"/>
+      <c r="BE51" s="11"/>
+      <c r="BF51" s="11"/>
+      <c r="BG51" s="11"/>
+      <c r="BH51" s="11"/>
+      <c r="BI51" s="4"/>
     </row>
-    <row r="52" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>359</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>13</v>
@@ -6548,8 +6898,8 @@
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="6"/>
-      <c r="J52" s="18" t="s">
-        <v>352</v>
+      <c r="J52" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="K52" s="5"/>
       <c r="L52" s="5" t="s">
@@ -6611,7 +6961,946 @@
       <c r="BB52" s="10"/>
       <c r="BC52" s="11"/>
       <c r="BD52" s="11"/>
-      <c r="BE52" s="4"/>
+      <c r="BE52" s="11"/>
+      <c r="BF52" s="11"/>
+      <c r="BG52" s="11"/>
+      <c r="BH52" s="11"/>
+      <c r="BI52" s="4"/>
+    </row>
+    <row r="53" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="H53" s="1"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="M53" s="4">
+        <v>278</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="O53" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="7"/>
+      <c r="X53" s="1"/>
+      <c r="Y53" s="1"/>
+      <c r="Z53" s="1"/>
+      <c r="AA53" s="1"/>
+      <c r="AB53" s="1"/>
+      <c r="AC53" s="1"/>
+      <c r="AD53" s="1"/>
+      <c r="AE53" s="1"/>
+      <c r="AF53" s="1"/>
+      <c r="AG53" s="1"/>
+      <c r="AH53" s="7"/>
+      <c r="AI53" s="1"/>
+      <c r="AJ53" s="1"/>
+      <c r="AK53" s="1"/>
+      <c r="AL53" s="1"/>
+      <c r="AM53" s="1"/>
+      <c r="AN53" s="1"/>
+      <c r="AO53" s="1"/>
+      <c r="AP53" s="1"/>
+      <c r="AQ53" s="1"/>
+      <c r="AR53" s="2"/>
+      <c r="AS53" s="9"/>
+      <c r="AT53" s="9"/>
+      <c r="AU53" s="9"/>
+      <c r="AV53" s="1"/>
+      <c r="AW53" s="1"/>
+      <c r="AX53" s="1"/>
+      <c r="AY53" s="1"/>
+      <c r="AZ53" s="1"/>
+      <c r="BA53" s="10"/>
+      <c r="BB53" s="10"/>
+      <c r="BC53" s="11"/>
+      <c r="BD53" s="11"/>
+      <c r="BE53" s="11"/>
+      <c r="BF53" s="11"/>
+      <c r="BG53" s="11"/>
+      <c r="BH53" s="11"/>
+      <c r="BI53" s="4"/>
+    </row>
+    <row r="54" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="H54" s="1"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="M54" s="4">
+        <v>278</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="O54" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="P54" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q54" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="R54" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="S54" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="T54" s="1"/>
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="7"/>
+      <c r="X54" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="Y54" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="Z54" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="AA54" s="1"/>
+      <c r="AB54" s="1"/>
+      <c r="AC54" s="1"/>
+      <c r="AD54" s="1"/>
+      <c r="AE54" s="1"/>
+      <c r="AF54" s="1"/>
+      <c r="AG54" s="1"/>
+      <c r="AH54" s="7"/>
+      <c r="AI54" s="1"/>
+      <c r="AJ54" s="1"/>
+      <c r="AK54" s="1"/>
+      <c r="AL54" s="1"/>
+      <c r="AM54" s="1"/>
+      <c r="AN54" s="1"/>
+      <c r="AO54" s="1"/>
+      <c r="AP54" s="1"/>
+      <c r="AQ54" s="1"/>
+      <c r="AR54" s="2"/>
+      <c r="AS54" s="9"/>
+      <c r="AT54" s="9"/>
+      <c r="AU54" s="9"/>
+      <c r="AV54" s="1"/>
+      <c r="AW54" s="1"/>
+      <c r="AX54" s="1"/>
+      <c r="AY54" s="1"/>
+      <c r="AZ54" s="1"/>
+      <c r="BA54" s="10"/>
+      <c r="BB54" s="10"/>
+      <c r="BC54" s="11"/>
+      <c r="BD54" s="11"/>
+      <c r="BE54" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="BF54" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="BG54" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="BH54" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="BI54" s="4"/>
+    </row>
+    <row r="55" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="H55" s="1"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="M55" s="4">
+        <v>278</v>
+      </c>
+      <c r="N55" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="O55" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="P55" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q55" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="R55" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="S55" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="T55" s="1"/>
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="W55" s="7"/>
+      <c r="X55" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="Y55" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="Z55" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="AA55" s="1"/>
+      <c r="AB55" s="1"/>
+      <c r="AC55" s="1"/>
+      <c r="AD55" s="1"/>
+      <c r="AE55" s="1"/>
+      <c r="AF55" s="1"/>
+      <c r="AG55" s="1"/>
+      <c r="AH55" s="7"/>
+      <c r="AI55" s="1"/>
+      <c r="AJ55" s="1"/>
+      <c r="AK55" s="1"/>
+      <c r="AL55" s="1"/>
+      <c r="AM55" s="1"/>
+      <c r="AN55" s="1"/>
+      <c r="AO55" s="1"/>
+      <c r="AP55" s="1"/>
+      <c r="AQ55" s="1"/>
+      <c r="AR55" s="2"/>
+      <c r="AS55" s="9"/>
+      <c r="AT55" s="9"/>
+      <c r="AU55" s="9"/>
+      <c r="AV55" s="1"/>
+      <c r="AW55" s="1"/>
+      <c r="AX55" s="1"/>
+      <c r="AY55" s="1"/>
+      <c r="AZ55" s="1"/>
+      <c r="BA55" s="10"/>
+      <c r="BB55" s="10"/>
+      <c r="BC55" s="11"/>
+      <c r="BD55" s="11"/>
+      <c r="BE55" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="BF55" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="BG55" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="BH55" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="BI55" s="4"/>
+    </row>
+    <row r="56" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="H56" s="1"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="M56" s="4">
+        <v>278</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="R56" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="S56" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="T56" s="1"/>
+      <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="W56" s="7"/>
+      <c r="X56" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="Y56" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="Z56" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="AA56" s="1"/>
+      <c r="AB56" s="1"/>
+      <c r="AC56" s="1"/>
+      <c r="AD56" s="1"/>
+      <c r="AE56" s="1"/>
+      <c r="AF56" s="1"/>
+      <c r="AG56" s="1"/>
+      <c r="AH56" s="7"/>
+      <c r="AI56" s="1"/>
+      <c r="AJ56" s="1"/>
+      <c r="AK56" s="1"/>
+      <c r="AL56" s="1"/>
+      <c r="AM56" s="1"/>
+      <c r="AN56" s="1"/>
+      <c r="AO56" s="1"/>
+      <c r="AP56" s="1"/>
+      <c r="AQ56" s="1"/>
+      <c r="AR56" s="2"/>
+      <c r="AS56" s="9"/>
+      <c r="AT56" s="9"/>
+      <c r="AU56" s="9"/>
+      <c r="AV56" s="1"/>
+      <c r="AW56" s="1"/>
+      <c r="AX56" s="1"/>
+      <c r="AY56" s="1"/>
+      <c r="AZ56" s="1"/>
+      <c r="BA56" s="10"/>
+      <c r="BB56" s="10"/>
+      <c r="BC56" s="11"/>
+      <c r="BD56" s="11"/>
+      <c r="BE56" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="BF56" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="BG56" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="BH56" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="BI56" s="4"/>
+    </row>
+    <row r="57" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="H57" s="1"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="M57" s="4">
+        <v>278</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="R57" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="S57" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="T57" s="1"/>
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="7"/>
+      <c r="X57" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="Y57" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="Z57" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="AA57" s="1"/>
+      <c r="AB57" s="1"/>
+      <c r="AC57" s="1"/>
+      <c r="AD57" s="1"/>
+      <c r="AE57" s="1"/>
+      <c r="AF57" s="1"/>
+      <c r="AG57" s="1"/>
+      <c r="AH57" s="7"/>
+      <c r="AI57" s="1"/>
+      <c r="AJ57" s="1"/>
+      <c r="AK57" s="1"/>
+      <c r="AL57" s="1"/>
+      <c r="AM57" s="1"/>
+      <c r="AN57" s="1"/>
+      <c r="AO57" s="1"/>
+      <c r="AP57" s="1"/>
+      <c r="AQ57" s="1"/>
+      <c r="AR57" s="2"/>
+      <c r="AS57" s="9"/>
+      <c r="AT57" s="9"/>
+      <c r="AU57" s="9"/>
+      <c r="AV57" s="1"/>
+      <c r="AW57" s="1"/>
+      <c r="AX57" s="1"/>
+      <c r="AY57" s="1"/>
+      <c r="AZ57" s="1"/>
+      <c r="BA57" s="10"/>
+      <c r="BB57" s="10"/>
+      <c r="BC57" s="11"/>
+      <c r="BD57" s="11"/>
+      <c r="BE57" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="BF57" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="BG57" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="BH57" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="BI57" s="4"/>
+    </row>
+    <row r="58" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="H58" s="1"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="M58" s="4">
+        <v>278</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q58" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="R58" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="S58" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="T58" s="1"/>
+      <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
+      <c r="W58" s="7"/>
+      <c r="X58" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="Y58" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="Z58" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="AA58" s="1"/>
+      <c r="AB58" s="1"/>
+      <c r="AC58" s="1"/>
+      <c r="AD58" s="1"/>
+      <c r="AE58" s="1"/>
+      <c r="AF58" s="1"/>
+      <c r="AG58" s="1"/>
+      <c r="AH58" s="7"/>
+      <c r="AI58" s="1"/>
+      <c r="AJ58" s="1"/>
+      <c r="AK58" s="1"/>
+      <c r="AL58" s="1"/>
+      <c r="AM58" s="1"/>
+      <c r="AN58" s="1"/>
+      <c r="AO58" s="1"/>
+      <c r="AP58" s="1"/>
+      <c r="AQ58" s="1"/>
+      <c r="AR58" s="2"/>
+      <c r="AS58" s="9"/>
+      <c r="AT58" s="9"/>
+      <c r="AU58" s="9"/>
+      <c r="AV58" s="1"/>
+      <c r="AW58" s="1"/>
+      <c r="AX58" s="1"/>
+      <c r="AY58" s="1"/>
+      <c r="AZ58" s="1"/>
+      <c r="BA58" s="10"/>
+      <c r="BB58" s="10"/>
+      <c r="BC58" s="11"/>
+      <c r="BD58" s="11"/>
+      <c r="BE58" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="BF58" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="BG58" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="BH58" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="BI58" s="4"/>
+    </row>
+    <row r="59" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="H59" s="1"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="M59" s="4">
+        <v>278</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q59" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="R59" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="S59" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="T59" s="1"/>
+      <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
+      <c r="W59" s="7"/>
+      <c r="X59" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="Y59" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="Z59" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="AA59" s="1"/>
+      <c r="AB59" s="1"/>
+      <c r="AC59" s="1"/>
+      <c r="AD59" s="1"/>
+      <c r="AE59" s="1"/>
+      <c r="AF59" s="1"/>
+      <c r="AG59" s="1"/>
+      <c r="AH59" s="7"/>
+      <c r="AI59" s="1"/>
+      <c r="AJ59" s="1"/>
+      <c r="AK59" s="1"/>
+      <c r="AL59" s="1"/>
+      <c r="AM59" s="1"/>
+      <c r="AN59" s="1"/>
+      <c r="AO59" s="1"/>
+      <c r="AP59" s="1"/>
+      <c r="AQ59" s="1"/>
+      <c r="AR59" s="2"/>
+      <c r="AS59" s="9"/>
+      <c r="AT59" s="9"/>
+      <c r="AU59" s="9"/>
+      <c r="AV59" s="1"/>
+      <c r="AW59" s="1"/>
+      <c r="AX59" s="1"/>
+      <c r="AY59" s="1"/>
+      <c r="AZ59" s="1"/>
+      <c r="BA59" s="10"/>
+      <c r="BB59" s="10"/>
+      <c r="BC59" s="11"/>
+      <c r="BD59" s="11"/>
+      <c r="BE59" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="BF59" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="BG59" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="BH59" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="BI59" s="4"/>
+    </row>
+    <row r="60" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="H60" s="1"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="M60" s="4">
+        <v>278</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q60" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="R60" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="S60" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="7"/>
+      <c r="X60" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="Y60" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="Z60" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="AA60" s="1"/>
+      <c r="AB60" s="1"/>
+      <c r="AC60" s="1"/>
+      <c r="AD60" s="1"/>
+      <c r="AE60" s="1"/>
+      <c r="AF60" s="1"/>
+      <c r="AG60" s="1"/>
+      <c r="AH60" s="7"/>
+      <c r="AI60" s="1"/>
+      <c r="AJ60" s="1"/>
+      <c r="AK60" s="1"/>
+      <c r="AL60" s="1"/>
+      <c r="AM60" s="1"/>
+      <c r="AN60" s="1"/>
+      <c r="AO60" s="1"/>
+      <c r="AP60" s="1"/>
+      <c r="AQ60" s="1"/>
+      <c r="AR60" s="2"/>
+      <c r="AS60" s="9"/>
+      <c r="AT60" s="9"/>
+      <c r="AU60" s="9"/>
+      <c r="AV60" s="1"/>
+      <c r="AW60" s="1"/>
+      <c r="AX60" s="1"/>
+      <c r="AY60" s="1"/>
+      <c r="AZ60" s="1"/>
+      <c r="BA60" s="10"/>
+      <c r="BB60" s="10"/>
+      <c r="BC60" s="11"/>
+      <c r="BD60" s="11"/>
+      <c r="BE60" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="BF60" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="BG60" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="BH60" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="BI60" s="4"/>
+    </row>
+    <row r="61" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="H61" s="1"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="M61" s="4">
+        <v>278</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="1"/>
+      <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
+      <c r="W61" s="7"/>
+      <c r="X61" s="1"/>
+      <c r="Y61" s="1"/>
+      <c r="Z61" s="1"/>
+      <c r="AA61" s="1"/>
+      <c r="AB61" s="1"/>
+      <c r="AC61" s="1"/>
+      <c r="AD61" s="1"/>
+      <c r="AE61" s="1"/>
+      <c r="AF61" s="1"/>
+      <c r="AG61" s="1"/>
+      <c r="AH61" s="7"/>
+      <c r="AI61" s="1"/>
+      <c r="AJ61" s="1"/>
+      <c r="AK61" s="1"/>
+      <c r="AL61" s="1"/>
+      <c r="AM61" s="1"/>
+      <c r="AN61" s="1"/>
+      <c r="AO61" s="1"/>
+      <c r="AP61" s="1"/>
+      <c r="AQ61" s="1"/>
+      <c r="AR61" s="2"/>
+      <c r="AS61" s="9"/>
+      <c r="AT61" s="9"/>
+      <c r="AU61" s="9"/>
+      <c r="AV61" s="1"/>
+      <c r="AW61" s="1"/>
+      <c r="AX61" s="1"/>
+      <c r="AY61" s="1"/>
+      <c r="AZ61" s="1"/>
+      <c r="BA61" s="10"/>
+      <c r="BB61" s="10"/>
+      <c r="BC61" s="11"/>
+      <c r="BD61" s="11"/>
+      <c r="BE61" s="11"/>
+      <c r="BF61" s="13"/>
+      <c r="BG61" s="14"/>
+      <c r="BH61" s="11"/>
+      <c r="BI61" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>